<commit_message>
US-1-updated tc review comments
</commit_message>
<xml_diff>
--- a/qa-mars-onboading-manual-tc/TC_Onboarding Task.xlsx
+++ b/qa-mars-onboading-manual-tc/TC_Onboarding Task.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/42a9bb15bec37803/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/42a9bb15bec37803/Documents/industryconnect_git_repos/qa-mars-repo/qa-mars-onboading-manual-tc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="759" documentId="8_{2E5F233C-7F86-4BF6-B4CC-5D124B90EC91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EA62DC97-6458-4AFF-B0DD-B8443ABE76E9}"/>
+  <xr:revisionPtr revIDLastSave="46" documentId="8_{8B28C1AA-7850-4101-AE68-A22D4683C709}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4CBEC567-A72E-49A6-BA6A-09425D0228C7}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{8E1C5F8A-1356-4823-A53B-F06F0170C2EE}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="3" activeTab="7" xr2:uid="{8E1C5F8A-1356-4823-A53B-F06F0170C2EE}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover Sheet" sheetId="3" r:id="rId1"/>
@@ -20,7 +20,8 @@
     <sheet name="Language_Test Cases" sheetId="8" r:id="rId5"/>
     <sheet name="Skills_Test Cases" sheetId="1" r:id="rId6"/>
     <sheet name="Data for Testing" sheetId="5" r:id="rId7"/>
-    <sheet name="Sheet6" sheetId="6" state="hidden" r:id="rId8"/>
+    <sheet name="Review Comments" sheetId="9" r:id="rId8"/>
+    <sheet name="Sheet6" sheetId="6" state="hidden" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="586" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="629" uniqueCount="190">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -237,11 +238,6 @@
     <t>User should be able to click on Join button</t>
   </si>
   <si>
-    <t xml:space="preserve">1. Open the Chrome brwoser and enter the url to launch the Mars Logo application .
- [Refer test data for Url]
-     </t>
-  </si>
-  <si>
     <t xml:space="preserve">3. Enter the valid data in the following input fields :
 First Name
 Last Name
@@ -295,9 +291,6 @@
     <t>TC003</t>
   </si>
   <si>
-    <t xml:space="preserve">To Verify if user is able to "Join" to Mars Logo application with invalid data </t>
-  </si>
-  <si>
     <t xml:space="preserve"> First Name - Dd
 Last Name - blank
 Email address - dhanushreeak2@gmail.com
@@ -433,9 +426,6 @@
     <t>TC007</t>
   </si>
   <si>
-    <t>To Verify if user is able to add the language in the Languages section under Profile page with invalid data</t>
-  </si>
-  <si>
     <t xml:space="preserve">8. Enter the invalid language in Add language textbox and  select the language level from the choose language level drop down </t>
   </si>
   <si>
@@ -604,9 +594,6 @@
 </t>
   </si>
   <si>
-    <t>To Verify if user is able to add a skill in the Skills section under Profile page with invalid data</t>
-  </si>
-  <si>
     <t xml:space="preserve">8. Enter the invalid skill in Add skill textbox and  select the skill level from the choose skill level drop down </t>
   </si>
   <si>
@@ -659,6 +646,62 @@
   </si>
   <si>
     <t>Error message should be displayed and user should not be able login to application</t>
+  </si>
+  <si>
+    <t>Please increase your coverage around the features you are testing here is an idea of what is missing 
+• Negative testing with valid input
+• Negative testing with invalid input
+• Destructive testing
+E.g of above scenarios
+Happy path tests check basic functionality and the acceptance criteria of the API. We later extend positive tests to include optional parameters and extra functionality.
+The next group of tests is negative testing where we expect the application to gracefully handle problem scenarios with both valid user input (for example, trying to add an existing username) and invalid user input (trying to add a username which is null).
+Destructive testing is a deeper form of negative testing where we intentionally attempt to break the API to check its robustness (for example, sending a huge payload body in an attempt to overflow the system).
+If some scenarios does not make sense to add you can you should know why it does not make sense to add.
+think about special characters, empty values, long text inputs etc
+you also need to thing about what happens delete language that does not exit
+update langauge that does not exist etc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Open the Chrome browser and enter the url to launch the Mars Logo application .
+ [Refer test data for Url]
+     </t>
+  </si>
+  <si>
+    <t>TC011</t>
+  </si>
+  <si>
+    <t>To Verify if user is able to update language which does not exist in the Languages section under Profile page</t>
+  </si>
+  <si>
+    <t>Language cannot be updated</t>
+  </si>
+  <si>
+    <t>To Verify if user is able to add the language in the Languages section under Profile page with invalid data(special characters,null value)</t>
+  </si>
+  <si>
+    <t>To Verify if user is able to "Join" to Mars Logo application with invalid data (special characters,null value)</t>
+  </si>
+  <si>
+    <t>To Verify if user is able to add a skill in the Skills section under Profile page with invalid data(special characters,null value)</t>
+  </si>
+  <si>
+    <t>To Verify if user is able to update skill which does not exist in the Skills section under Profile page</t>
+  </si>
+  <si>
+    <t>7. Edit the Skill details which does not exist in the Skill list</t>
+  </si>
+  <si>
+    <t>skill - Python
+Level- Expert</t>
+  </si>
+  <si>
+    <t>Skill cannot be updated</t>
+  </si>
+  <si>
+    <t>7. Edit the language details which does not exist in the languages list</t>
+  </si>
+  <si>
+    <t>Updated the test cases as per the review comments</t>
   </si>
 </sst>
 </file>
@@ -829,7 +872,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -898,28 +941,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -932,20 +956,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -960,8 +975,26 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1411,8 +1444,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6C9E9E2-0D3F-4DF3-BF6D-07E5DA17B63E}">
   <dimension ref="A1:C24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1422,7 +1455,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="36" t="s">
         <v>37</v>
       </c>
       <c r="B1" s="22" t="s">
@@ -1433,16 +1466,16 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="24"/>
+      <c r="A2" s="36"/>
       <c r="B2" s="18" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C2" s="19" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="24"/>
+      <c r="A3" s="36"/>
       <c r="B3" s="18" t="s">
         <v>28</v>
       </c>
@@ -1451,16 +1484,16 @@
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="24"/>
+      <c r="A4" s="36"/>
       <c r="B4" s="18" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C4" s="19" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="24"/>
+      <c r="A5" s="36"/>
       <c r="B5" s="18" t="s">
         <v>22</v>
       </c>
@@ -1469,7 +1502,7 @@
       </c>
     </row>
     <row r="6" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A6" s="24" t="s">
+      <c r="A6" s="36" t="s">
         <v>38</v>
       </c>
       <c r="B6" s="18" t="s">
@@ -1480,7 +1513,7 @@
       </c>
     </row>
     <row r="7" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A7" s="24"/>
+      <c r="A7" s="36"/>
       <c r="B7" s="18" t="s">
         <v>26</v>
       </c>
@@ -1489,7 +1522,7 @@
       </c>
     </row>
     <row r="8" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A8" s="24"/>
+      <c r="A8" s="36"/>
       <c r="B8" s="18" t="s">
         <v>23</v>
       </c>
@@ -1498,7 +1531,7 @@
       </c>
     </row>
     <row r="9" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A9" s="24"/>
+      <c r="A9" s="36"/>
       <c r="B9" s="18" t="s">
         <v>29</v>
       </c>
@@ -1507,7 +1540,7 @@
       </c>
     </row>
     <row r="10" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A10" s="24"/>
+      <c r="A10" s="36"/>
       <c r="B10" s="18" t="s">
         <v>30</v>
       </c>
@@ -1516,16 +1549,16 @@
       </c>
     </row>
     <row r="11" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A11" s="24"/>
+      <c r="A11" s="36"/>
       <c r="B11" s="18" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="C11" s="19" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A12" s="24"/>
+      <c r="A12" s="36"/>
       <c r="B12" s="18" t="s">
         <v>31</v>
       </c>
@@ -1534,7 +1567,7 @@
       </c>
     </row>
     <row r="13" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A13" s="24"/>
+      <c r="A13" s="36"/>
       <c r="B13" s="18" t="s">
         <v>32</v>
       </c>
@@ -1543,16 +1576,16 @@
       </c>
     </row>
     <row r="14" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A14" s="24"/>
+      <c r="A14" s="36"/>
       <c r="B14" s="18" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C14" s="19" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A15" s="24"/>
+      <c r="A15" s="36"/>
       <c r="B15" s="18" t="s">
         <v>25</v>
       </c>
@@ -1561,7 +1594,7 @@
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A16" s="24" t="s">
+      <c r="A16" s="36" t="s">
         <v>46</v>
       </c>
       <c r="B16" s="18" t="s">
@@ -1572,7 +1605,7 @@
       </c>
     </row>
     <row r="17" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A17" s="24"/>
+      <c r="A17" s="36"/>
       <c r="B17" s="18" t="s">
         <v>40</v>
       </c>
@@ -1581,7 +1614,7 @@
       </c>
     </row>
     <row r="18" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A18" s="24"/>
+      <c r="A18" s="36"/>
       <c r="B18" s="18" t="s">
         <v>41</v>
       </c>
@@ -1590,7 +1623,7 @@
       </c>
     </row>
     <row r="19" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A19" s="24"/>
+      <c r="A19" s="36"/>
       <c r="B19" s="18" t="s">
         <v>42</v>
       </c>
@@ -1599,7 +1632,7 @@
       </c>
     </row>
     <row r="20" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A20" s="24"/>
+      <c r="A20" s="36"/>
       <c r="B20" s="18" t="s">
         <v>43</v>
       </c>
@@ -1608,17 +1641,17 @@
       </c>
     </row>
     <row r="21" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A21" s="24"/>
+      <c r="A21" s="36"/>
       <c r="B21" s="18" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="C21" s="19" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A22" s="24"/>
-      <c r="B22" s="39" t="s">
+      <c r="A22" s="36"/>
+      <c r="B22" s="30" t="s">
         <v>44</v>
       </c>
       <c r="C22" s="19" t="s">
@@ -1626,7 +1659,7 @@
       </c>
     </row>
     <row r="23" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A23" s="24"/>
+      <c r="A23" s="36"/>
       <c r="B23" s="18" t="s">
         <v>45</v>
       </c>
@@ -1635,9 +1668,9 @@
       </c>
     </row>
     <row r="24" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A24" s="24"/>
+      <c r="A24" s="36"/>
       <c r="B24" s="18" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="C24" s="19" t="s">
         <v>34</v>
@@ -1657,8 +1690,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04703EE0-2DC8-480A-B8AF-8B36161CC0E5}">
   <dimension ref="A1:J22"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10:B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1708,20 +1741,20 @@
       </c>
     </row>
     <row r="2" spans="1:10" s="1" customFormat="1" ht="43.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="28" t="s">
+      <c r="A2" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="28" t="s">
+      <c r="B2" s="37" t="s">
         <v>53</v>
       </c>
-      <c r="C2" s="28" t="s">
+      <c r="C2" s="37" t="s">
         <v>56</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>60</v>
+        <v>177</v>
       </c>
       <c r="E2" s="21" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F2" s="18" t="s">
         <v>55</v>
@@ -1732,9 +1765,9 @@
       <c r="J2" s="2"/>
     </row>
     <row r="3" spans="1:10" s="1" customFormat="1" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="28"/>
-      <c r="B3" s="28"/>
-      <c r="C3" s="28"/>
+      <c r="A3" s="37"/>
+      <c r="B3" s="37"/>
+      <c r="C3" s="37"/>
       <c r="D3" s="18" t="s">
         <v>54</v>
       </c>
@@ -1748,11 +1781,11 @@
       <c r="J3" s="19"/>
     </row>
     <row r="4" spans="1:10" ht="120" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="28"/>
-      <c r="B4" s="28"/>
-      <c r="C4" s="28"/>
+      <c r="A4" s="37"/>
+      <c r="B4" s="37"/>
+      <c r="C4" s="37"/>
       <c r="D4" s="22" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E4" s="18" t="s">
         <v>51</v>
@@ -1766,9 +1799,9 @@
       <c r="J4" s="20"/>
     </row>
     <row r="5" spans="1:10" s="1" customFormat="1" ht="34.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="28"/>
-      <c r="B5" s="28"/>
-      <c r="C5" s="28"/>
+      <c r="A5" s="37"/>
+      <c r="B5" s="37"/>
+      <c r="C5" s="37"/>
       <c r="D5" s="19" t="s">
         <v>58</v>
       </c>
@@ -1782,20 +1815,20 @@
       <c r="J5" s="19"/>
     </row>
     <row r="6" spans="1:10" s="1" customFormat="1" ht="46.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="28" t="s">
+      <c r="A6" s="37" t="s">
         <v>52</v>
       </c>
-      <c r="B6" s="28" t="s">
-        <v>63</v>
-      </c>
-      <c r="C6" s="28" t="s">
+      <c r="B6" s="37" t="s">
+        <v>62</v>
+      </c>
+      <c r="C6" s="37" t="s">
         <v>56</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>60</v>
+        <v>177</v>
       </c>
       <c r="E6" s="18" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F6" s="18" t="s">
         <v>55</v>
@@ -1806,15 +1839,15 @@
       <c r="J6" s="19"/>
     </row>
     <row r="7" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A7" s="28"/>
-      <c r="B7" s="28"/>
-      <c r="C7" s="28"/>
+      <c r="A7" s="37"/>
+      <c r="B7" s="37"/>
+      <c r="C7" s="37"/>
       <c r="D7" s="22" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E7" s="20"/>
       <c r="F7" s="18" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G7" s="20"/>
       <c r="H7" s="20"/>
@@ -1822,17 +1855,17 @@
       <c r="J7" s="20"/>
     </row>
     <row r="8" spans="1:10" ht="72" x14ac:dyDescent="0.3">
-      <c r="A8" s="28"/>
-      <c r="B8" s="28"/>
-      <c r="C8" s="28"/>
+      <c r="A8" s="37"/>
+      <c r="B8" s="37"/>
+      <c r="C8" s="37"/>
       <c r="D8" s="22" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E8" s="18" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F8" s="18" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G8" s="20"/>
       <c r="H8" s="20"/>
@@ -1840,15 +1873,15 @@
       <c r="J8" s="20"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A9" s="28"/>
-      <c r="B9" s="28"/>
-      <c r="C9" s="28"/>
+      <c r="A9" s="37"/>
+      <c r="B9" s="37"/>
+      <c r="C9" s="37"/>
       <c r="D9" s="22" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E9" s="20"/>
       <c r="F9" s="20" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G9" s="20"/>
       <c r="H9" s="20"/>
@@ -1856,20 +1889,20 @@
       <c r="J9" s="20"/>
     </row>
     <row r="10" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A10" s="28" t="s">
-        <v>73</v>
-      </c>
-      <c r="B10" s="28" t="s">
-        <v>74</v>
-      </c>
-      <c r="C10" s="28" t="s">
+      <c r="A10" s="37" t="s">
+        <v>72</v>
+      </c>
+      <c r="B10" s="37" t="s">
+        <v>182</v>
+      </c>
+      <c r="C10" s="37" t="s">
         <v>56</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>60</v>
+        <v>177</v>
       </c>
       <c r="E10" s="21" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F10" s="18" t="s">
         <v>55</v>
@@ -1880,9 +1913,9 @@
       <c r="J10" s="20"/>
     </row>
     <row r="11" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A11" s="28"/>
-      <c r="B11" s="28"/>
-      <c r="C11" s="28"/>
+      <c r="A11" s="37"/>
+      <c r="B11" s="37"/>
+      <c r="C11" s="37"/>
       <c r="D11" s="18" t="s">
         <v>54</v>
       </c>
@@ -1896,14 +1929,14 @@
       <c r="J11" s="20"/>
     </row>
     <row r="12" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="A12" s="28"/>
-      <c r="B12" s="28"/>
-      <c r="C12" s="28"/>
+      <c r="A12" s="37"/>
+      <c r="B12" s="37"/>
+      <c r="C12" s="37"/>
       <c r="D12" s="22" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E12" s="18" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F12" s="18" t="s">
         <v>57</v>
@@ -1914,15 +1947,15 @@
       <c r="J12" s="20"/>
     </row>
     <row r="13" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A13" s="28"/>
-      <c r="B13" s="28"/>
-      <c r="C13" s="28"/>
+      <c r="A13" s="37"/>
+      <c r="B13" s="37"/>
+      <c r="C13" s="37"/>
       <c r="D13" s="19" t="s">
         <v>58</v>
       </c>
       <c r="E13" s="18"/>
       <c r="F13" s="2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="G13" s="20"/>
       <c r="H13" s="20"/>
@@ -1930,20 +1963,20 @@
       <c r="J13" s="20"/>
     </row>
     <row r="14" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A14" s="28" t="s">
-        <v>78</v>
-      </c>
-      <c r="B14" s="28" t="s">
-        <v>79</v>
-      </c>
-      <c r="C14" s="28" t="s">
+      <c r="A14" s="37" t="s">
+        <v>76</v>
+      </c>
+      <c r="B14" s="37" t="s">
+        <v>77</v>
+      </c>
+      <c r="C14" s="37" t="s">
         <v>56</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>60</v>
+        <v>177</v>
       </c>
       <c r="E14" s="18" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F14" s="18" t="s">
         <v>55</v>
@@ -1954,15 +1987,15 @@
       <c r="J14" s="20"/>
     </row>
     <row r="15" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A15" s="28"/>
-      <c r="B15" s="28"/>
-      <c r="C15" s="28"/>
+      <c r="A15" s="37"/>
+      <c r="B15" s="37"/>
+      <c r="C15" s="37"/>
       <c r="D15" s="22" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E15" s="20"/>
       <c r="F15" s="18" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G15" s="20"/>
       <c r="H15" s="20"/>
@@ -1970,17 +2003,17 @@
       <c r="J15" s="20"/>
     </row>
     <row r="16" spans="1:10" ht="72" x14ac:dyDescent="0.3">
-      <c r="A16" s="28"/>
-      <c r="B16" s="28"/>
-      <c r="C16" s="28"/>
+      <c r="A16" s="37"/>
+      <c r="B16" s="37"/>
+      <c r="C16" s="37"/>
       <c r="D16" s="22" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E16" s="18" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="F16" s="18" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G16" s="20"/>
       <c r="H16" s="20"/>
@@ -1988,15 +2021,15 @@
       <c r="J16" s="20"/>
     </row>
     <row r="17" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A17" s="28"/>
-      <c r="B17" s="28"/>
-      <c r="C17" s="28"/>
+      <c r="A17" s="37"/>
+      <c r="B17" s="37"/>
+      <c r="C17" s="37"/>
       <c r="D17" s="22" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E17" s="20"/>
       <c r="F17" s="22" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="G17" s="20"/>
       <c r="H17" s="20"/>
@@ -2004,20 +2037,20 @@
       <c r="J17" s="20"/>
     </row>
     <row r="18" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A18" s="28" t="s">
-        <v>106</v>
-      </c>
-      <c r="B18" s="28" t="s">
-        <v>176</v>
-      </c>
-      <c r="C18" s="28" t="s">
+      <c r="A18" s="37" t="s">
+        <v>104</v>
+      </c>
+      <c r="B18" s="37" t="s">
+        <v>172</v>
+      </c>
+      <c r="C18" s="37" t="s">
         <v>56</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>60</v>
+        <v>177</v>
       </c>
       <c r="E18" s="18" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F18" s="18" t="s">
         <v>55</v>
@@ -2028,15 +2061,15 @@
       <c r="J18" s="20"/>
     </row>
     <row r="19" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A19" s="28"/>
-      <c r="B19" s="28"/>
-      <c r="C19" s="28"/>
+      <c r="A19" s="37"/>
+      <c r="B19" s="37"/>
+      <c r="C19" s="37"/>
       <c r="D19" s="22" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E19" s="20"/>
       <c r="F19" s="18" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G19" s="20"/>
       <c r="H19" s="20"/>
@@ -2044,17 +2077,17 @@
       <c r="J19" s="20"/>
     </row>
     <row r="20" spans="1:10" ht="72" x14ac:dyDescent="0.3">
-      <c r="A20" s="28"/>
-      <c r="B20" s="28"/>
-      <c r="C20" s="28"/>
+      <c r="A20" s="37"/>
+      <c r="B20" s="37"/>
+      <c r="C20" s="37"/>
       <c r="D20" s="22" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E20" s="18" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F20" s="18" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G20" s="20"/>
       <c r="H20" s="20"/>
@@ -2062,15 +2095,15 @@
       <c r="J20" s="20"/>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A21" s="28"/>
-      <c r="B21" s="28"/>
-      <c r="C21" s="28"/>
+      <c r="A21" s="37"/>
+      <c r="B21" s="37"/>
+      <c r="C21" s="37"/>
       <c r="D21" s="22" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E21" s="20"/>
       <c r="F21" s="20" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G21" s="20"/>
       <c r="H21" s="20"/>
@@ -2078,15 +2111,15 @@
       <c r="J21" s="20"/>
     </row>
     <row r="22" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A22" s="28"/>
-      <c r="B22" s="28"/>
-      <c r="C22" s="28"/>
-      <c r="D22" s="46" t="s">
-        <v>177</v>
+      <c r="A22" s="37"/>
+      <c r="B22" s="37"/>
+      <c r="C22" s="37"/>
+      <c r="D22" s="22" t="s">
+        <v>173</v>
       </c>
       <c r="E22" s="20"/>
       <c r="F22" s="22" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="G22" s="20"/>
       <c r="H22" s="20"/>
@@ -2118,10 +2151,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA34FC2A-DA0E-47B6-BE06-C2F4AAE7B6C8}">
-  <dimension ref="A1:J81"/>
+  <dimension ref="A1:J88"/>
   <sheetViews>
-    <sheetView topLeftCell="A74" workbookViewId="0">
-      <selection activeCell="A74" sqref="A74:A80"/>
+    <sheetView topLeftCell="A80" workbookViewId="0">
+      <selection activeCell="C88" sqref="C87:F88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2171,20 +2204,20 @@
       </c>
     </row>
     <row r="2" spans="1:10" s="1" customFormat="1" ht="47.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="28" t="s">
+      <c r="A2" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="28" t="s">
-        <v>82</v>
-      </c>
-      <c r="C2" s="28" t="s">
+      <c r="B2" s="37" t="s">
+        <v>80</v>
+      </c>
+      <c r="C2" s="37" t="s">
         <v>56</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>60</v>
+        <v>177</v>
       </c>
       <c r="E2" s="18" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F2" s="18" t="s">
         <v>55</v>
@@ -2195,15 +2228,15 @@
       <c r="J2" s="2"/>
     </row>
     <row r="3" spans="1:10" s="1" customFormat="1" ht="30.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="28"/>
-      <c r="B3" s="28"/>
-      <c r="C3" s="28"/>
+      <c r="A3" s="37"/>
+      <c r="B3" s="37"/>
+      <c r="C3" s="37"/>
       <c r="D3" s="18" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E3" s="19"/>
       <c r="F3" s="18" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G3" s="19"/>
       <c r="H3" s="19"/>
@@ -2211,17 +2244,17 @@
       <c r="J3" s="19"/>
     </row>
     <row r="4" spans="1:10" ht="60" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="28"/>
-      <c r="B4" s="28"/>
-      <c r="C4" s="28"/>
+      <c r="A4" s="37"/>
+      <c r="B4" s="37"/>
+      <c r="C4" s="37"/>
       <c r="D4" s="18" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E4" s="18" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F4" s="18" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G4" s="20"/>
       <c r="H4" s="20"/>
@@ -2229,15 +2262,15 @@
       <c r="J4" s="20"/>
     </row>
     <row r="5" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A5" s="28"/>
-      <c r="B5" s="28"/>
-      <c r="C5" s="28"/>
+      <c r="A5" s="37"/>
+      <c r="B5" s="37"/>
+      <c r="C5" s="37"/>
       <c r="D5" s="22" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E5" s="20"/>
       <c r="F5" s="22" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G5" s="20"/>
       <c r="H5" s="20"/>
@@ -2245,15 +2278,15 @@
       <c r="J5" s="20"/>
     </row>
     <row r="6" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A6" s="28"/>
-      <c r="B6" s="28"/>
-      <c r="C6" s="28"/>
+      <c r="A6" s="37"/>
+      <c r="B6" s="37"/>
+      <c r="C6" s="37"/>
       <c r="D6" s="20" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E6" s="20"/>
       <c r="F6" s="22" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="G6" s="20"/>
       <c r="H6" s="20"/>
@@ -2261,15 +2294,15 @@
       <c r="J6" s="20"/>
     </row>
     <row r="7" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A7" s="28"/>
-      <c r="B7" s="28"/>
-      <c r="C7" s="28"/>
+      <c r="A7" s="37"/>
+      <c r="B7" s="37"/>
+      <c r="C7" s="37"/>
       <c r="D7" s="20" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E7" s="20"/>
       <c r="F7" s="22" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="G7" s="20"/>
       <c r="H7" s="20"/>
@@ -2277,15 +2310,15 @@
       <c r="J7" s="20"/>
     </row>
     <row r="8" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A8" s="28"/>
-      <c r="B8" s="28"/>
-      <c r="C8" s="28"/>
+      <c r="A8" s="37"/>
+      <c r="B8" s="37"/>
+      <c r="C8" s="37"/>
       <c r="D8" s="20" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E8" s="20"/>
       <c r="F8" s="22" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="G8" s="20"/>
       <c r="H8" s="20"/>
@@ -2293,17 +2326,17 @@
       <c r="J8" s="20"/>
     </row>
     <row r="9" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A9" s="28"/>
-      <c r="B9" s="28"/>
-      <c r="C9" s="28"/>
+      <c r="A9" s="37"/>
+      <c r="B9" s="37"/>
+      <c r="C9" s="37"/>
       <c r="D9" s="22" t="s">
-        <v>88</v>
-      </c>
-      <c r="E9" s="35" t="s">
-        <v>118</v>
+        <v>86</v>
+      </c>
+      <c r="E9" s="28" t="s">
+        <v>115</v>
       </c>
       <c r="F9" s="22" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="G9" s="20"/>
       <c r="H9" s="20"/>
@@ -2311,15 +2344,15 @@
       <c r="J9" s="20"/>
     </row>
     <row r="10" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A10" s="28"/>
-      <c r="B10" s="28"/>
-      <c r="C10" s="28"/>
+      <c r="A10" s="37"/>
+      <c r="B10" s="37"/>
+      <c r="C10" s="37"/>
       <c r="D10" s="20" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E10" s="20"/>
       <c r="F10" s="22" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="G10" s="20"/>
       <c r="H10" s="20"/>
@@ -2327,20 +2360,20 @@
       <c r="J10" s="20"/>
     </row>
     <row r="11" spans="1:10" ht="72" x14ac:dyDescent="0.3">
-      <c r="A11" s="28" t="s">
+      <c r="A11" s="37" t="s">
         <v>52</v>
       </c>
-      <c r="B11" s="28" t="s">
-        <v>93</v>
-      </c>
-      <c r="C11" s="28" t="s">
+      <c r="B11" s="37" t="s">
+        <v>91</v>
+      </c>
+      <c r="C11" s="37" t="s">
         <v>56</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>60</v>
+        <v>177</v>
       </c>
       <c r="E11" s="18" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F11" s="18" t="s">
         <v>55</v>
@@ -2351,15 +2384,15 @@
       <c r="J11" s="20"/>
     </row>
     <row r="12" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A12" s="28"/>
-      <c r="B12" s="28"/>
-      <c r="C12" s="28"/>
+      <c r="A12" s="37"/>
+      <c r="B12" s="37"/>
+      <c r="C12" s="37"/>
       <c r="D12" s="18" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E12" s="19"/>
       <c r="F12" s="18" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G12" s="20"/>
       <c r="H12" s="20"/>
@@ -2367,17 +2400,17 @@
       <c r="J12" s="20"/>
     </row>
     <row r="13" spans="1:10" ht="72" x14ac:dyDescent="0.3">
-      <c r="A13" s="28"/>
-      <c r="B13" s="28"/>
-      <c r="C13" s="28"/>
+      <c r="A13" s="37"/>
+      <c r="B13" s="37"/>
+      <c r="C13" s="37"/>
       <c r="D13" s="18" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E13" s="18" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F13" s="18" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G13" s="20"/>
       <c r="H13" s="20"/>
@@ -2385,15 +2418,15 @@
       <c r="J13" s="20"/>
     </row>
     <row r="14" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A14" s="28"/>
-      <c r="B14" s="28"/>
-      <c r="C14" s="28"/>
+      <c r="A14" s="37"/>
+      <c r="B14" s="37"/>
+      <c r="C14" s="37"/>
       <c r="D14" s="22" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E14" s="20"/>
       <c r="F14" s="22" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G14" s="20"/>
       <c r="H14" s="20"/>
@@ -2401,15 +2434,15 @@
       <c r="J14" s="20"/>
     </row>
     <row r="15" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A15" s="28"/>
-      <c r="B15" s="28"/>
-      <c r="C15" s="28"/>
+      <c r="A15" s="37"/>
+      <c r="B15" s="37"/>
+      <c r="C15" s="37"/>
       <c r="D15" s="20" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E15" s="20"/>
       <c r="F15" s="22" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="G15" s="20"/>
       <c r="H15" s="20"/>
@@ -2417,15 +2450,15 @@
       <c r="J15" s="20"/>
     </row>
     <row r="16" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A16" s="28"/>
-      <c r="B16" s="28"/>
-      <c r="C16" s="28"/>
+      <c r="A16" s="37"/>
+      <c r="B16" s="37"/>
+      <c r="C16" s="37"/>
       <c r="D16" s="20" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E16" s="20"/>
       <c r="F16" s="22" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="G16" s="20"/>
       <c r="H16" s="20"/>
@@ -2433,19 +2466,19 @@
       <c r="J16" s="20"/>
     </row>
     <row r="17" spans="1:10" s="1" customFormat="1" ht="47.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="28"/>
-      <c r="B17" s="28"/>
-      <c r="C17" s="32" t="s">
-        <v>95</v>
+      <c r="A17" s="37"/>
+      <c r="B17" s="37"/>
+      <c r="C17" s="25" t="s">
+        <v>93</v>
       </c>
       <c r="D17" s="19" t="s">
-        <v>94</v>
-      </c>
-      <c r="E17" s="35" t="s">
-        <v>117</v>
+        <v>92</v>
+      </c>
+      <c r="E17" s="28" t="s">
+        <v>114</v>
       </c>
       <c r="F17" s="18" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="G17" s="19"/>
       <c r="H17" s="19"/>
@@ -2453,36 +2486,36 @@
       <c r="J17" s="19"/>
     </row>
     <row r="18" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A18" s="28"/>
-      <c r="B18" s="28"/>
-      <c r="C18" s="29"/>
+      <c r="A18" s="37"/>
+      <c r="B18" s="37"/>
+      <c r="C18" s="24"/>
       <c r="D18" s="20" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="E18" s="20"/>
       <c r="F18" s="22" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="G18" s="20"/>
       <c r="H18" s="20"/>
       <c r="I18" s="20"/>
       <c r="J18" s="20"/>
     </row>
-    <row r="19" spans="1:10" s="31" customFormat="1" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="25" t="s">
-        <v>73</v>
-      </c>
-      <c r="B19" s="25" t="s">
-        <v>99</v>
-      </c>
-      <c r="C19" s="28" t="s">
+    <row r="19" spans="1:10" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="38" t="s">
+        <v>72</v>
+      </c>
+      <c r="B19" s="38" t="s">
+        <v>97</v>
+      </c>
+      <c r="C19" s="37" t="s">
         <v>56</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>60</v>
+        <v>177</v>
       </c>
       <c r="E19" s="18" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F19" s="18" t="s">
         <v>55</v>
@@ -2493,15 +2526,15 @@
       <c r="J19" s="20"/>
     </row>
     <row r="20" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A20" s="26"/>
-      <c r="B20" s="26"/>
-      <c r="C20" s="28"/>
+      <c r="A20" s="39"/>
+      <c r="B20" s="39"/>
+      <c r="C20" s="37"/>
       <c r="D20" s="18" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E20" s="19"/>
       <c r="F20" s="18" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G20" s="20"/>
       <c r="H20" s="20"/>
@@ -2509,17 +2542,17 @@
       <c r="J20" s="20"/>
     </row>
     <row r="21" spans="1:10" ht="72" x14ac:dyDescent="0.3">
-      <c r="A21" s="26"/>
-      <c r="B21" s="26"/>
-      <c r="C21" s="28"/>
+      <c r="A21" s="39"/>
+      <c r="B21" s="39"/>
+      <c r="C21" s="37"/>
       <c r="D21" s="18" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E21" s="18" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F21" s="18" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G21" s="20"/>
       <c r="H21" s="20"/>
@@ -2527,15 +2560,15 @@
       <c r="J21" s="20"/>
     </row>
     <row r="22" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A22" s="26"/>
-      <c r="B22" s="26"/>
-      <c r="C22" s="28"/>
+      <c r="A22" s="39"/>
+      <c r="B22" s="39"/>
+      <c r="C22" s="37"/>
       <c r="D22" s="22" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E22" s="20"/>
       <c r="F22" s="22" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G22" s="20"/>
       <c r="H22" s="20"/>
@@ -2543,15 +2576,15 @@
       <c r="J22" s="20"/>
     </row>
     <row r="23" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A23" s="26"/>
-      <c r="B23" s="26"/>
-      <c r="C23" s="28"/>
+      <c r="A23" s="39"/>
+      <c r="B23" s="39"/>
+      <c r="C23" s="37"/>
       <c r="D23" s="20" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E23" s="20"/>
       <c r="F23" s="22" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="G23" s="20"/>
       <c r="H23" s="20"/>
@@ -2559,15 +2592,15 @@
       <c r="J23" s="20"/>
     </row>
     <row r="24" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A24" s="26"/>
-      <c r="B24" s="26"/>
-      <c r="C24" s="28"/>
+      <c r="A24" s="39"/>
+      <c r="B24" s="39"/>
+      <c r="C24" s="37"/>
       <c r="D24" s="20" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E24" s="20"/>
       <c r="F24" s="22" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="G24" s="20"/>
       <c r="H24" s="20"/>
@@ -2575,19 +2608,19 @@
       <c r="J24" s="20"/>
     </row>
     <row r="25" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A25" s="27"/>
-      <c r="B25" s="27"/>
-      <c r="C25" s="33" t="s">
-        <v>95</v>
-      </c>
-      <c r="D25" s="34" t="s">
-        <v>100</v>
-      </c>
-      <c r="E25" s="35" t="s">
-        <v>117</v>
-      </c>
-      <c r="F25" s="35" t="s">
-        <v>101</v>
+      <c r="A25" s="40"/>
+      <c r="B25" s="40"/>
+      <c r="C25" s="26" t="s">
+        <v>93</v>
+      </c>
+      <c r="D25" s="27" t="s">
+        <v>98</v>
+      </c>
+      <c r="E25" s="28" t="s">
+        <v>114</v>
+      </c>
+      <c r="F25" s="28" t="s">
+        <v>99</v>
       </c>
       <c r="G25" s="20"/>
       <c r="H25" s="20"/>
@@ -2595,20 +2628,20 @@
       <c r="J25" s="20"/>
     </row>
     <row r="26" spans="1:10" ht="72" x14ac:dyDescent="0.3">
-      <c r="A26" s="28" t="s">
-        <v>78</v>
-      </c>
-      <c r="B26" s="28" t="s">
-        <v>102</v>
-      </c>
-      <c r="C26" s="28" t="s">
+      <c r="A26" s="37" t="s">
+        <v>76</v>
+      </c>
+      <c r="B26" s="37" t="s">
+        <v>100</v>
+      </c>
+      <c r="C26" s="37" t="s">
         <v>56</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>60</v>
+        <v>177</v>
       </c>
       <c r="E26" s="18" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F26" s="18" t="s">
         <v>55</v>
@@ -2619,15 +2652,15 @@
       <c r="J26" s="20"/>
     </row>
     <row r="27" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A27" s="28"/>
-      <c r="B27" s="28"/>
-      <c r="C27" s="28"/>
+      <c r="A27" s="37"/>
+      <c r="B27" s="37"/>
+      <c r="C27" s="37"/>
       <c r="D27" s="18" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E27" s="19"/>
       <c r="F27" s="18" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G27" s="20"/>
       <c r="H27" s="20"/>
@@ -2635,17 +2668,17 @@
       <c r="J27" s="20"/>
     </row>
     <row r="28" spans="1:10" ht="72" x14ac:dyDescent="0.3">
-      <c r="A28" s="28"/>
-      <c r="B28" s="28"/>
-      <c r="C28" s="28"/>
+      <c r="A28" s="37"/>
+      <c r="B28" s="37"/>
+      <c r="C28" s="37"/>
       <c r="D28" s="18" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E28" s="18" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F28" s="18" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G28" s="20"/>
       <c r="H28" s="20"/>
@@ -2653,15 +2686,15 @@
       <c r="J28" s="20"/>
     </row>
     <row r="29" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A29" s="28"/>
-      <c r="B29" s="28"/>
-      <c r="C29" s="28"/>
+      <c r="A29" s="37"/>
+      <c r="B29" s="37"/>
+      <c r="C29" s="37"/>
       <c r="D29" s="22" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E29" s="20"/>
       <c r="F29" s="22" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G29" s="20"/>
       <c r="H29" s="20"/>
@@ -2669,15 +2702,15 @@
       <c r="J29" s="20"/>
     </row>
     <row r="30" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A30" s="28"/>
-      <c r="B30" s="28"/>
-      <c r="C30" s="28"/>
+      <c r="A30" s="37"/>
+      <c r="B30" s="37"/>
+      <c r="C30" s="37"/>
       <c r="D30" s="20" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E30" s="20"/>
       <c r="F30" s="22" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="G30" s="20"/>
       <c r="H30" s="20"/>
@@ -2685,15 +2718,15 @@
       <c r="J30" s="20"/>
     </row>
     <row r="31" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A31" s="28"/>
-      <c r="B31" s="28"/>
-      <c r="C31" s="28"/>
+      <c r="A31" s="37"/>
+      <c r="B31" s="37"/>
+      <c r="C31" s="37"/>
       <c r="D31" s="20" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E31" s="20"/>
       <c r="F31" s="22" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="G31" s="20"/>
       <c r="H31" s="20"/>
@@ -2701,15 +2734,15 @@
       <c r="J31" s="20"/>
     </row>
     <row r="32" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A32" s="28"/>
-      <c r="B32" s="28"/>
-      <c r="C32" s="28"/>
+      <c r="A32" s="37"/>
+      <c r="B32" s="37"/>
+      <c r="C32" s="37"/>
       <c r="D32" s="20" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E32" s="20"/>
       <c r="F32" s="22" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="G32" s="20"/>
       <c r="H32" s="20"/>
@@ -2717,17 +2750,17 @@
       <c r="J32" s="20"/>
     </row>
     <row r="33" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A33" s="28"/>
-      <c r="B33" s="28"/>
-      <c r="C33" s="28"/>
+      <c r="A33" s="37"/>
+      <c r="B33" s="37"/>
+      <c r="C33" s="37"/>
       <c r="D33" s="22" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="E33" s="21" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="F33" s="22" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="G33" s="20"/>
       <c r="H33" s="20"/>
@@ -2735,15 +2768,15 @@
       <c r="J33" s="20"/>
     </row>
     <row r="34" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A34" s="28"/>
-      <c r="B34" s="28"/>
-      <c r="C34" s="28"/>
+      <c r="A34" s="37"/>
+      <c r="B34" s="37"/>
+      <c r="C34" s="37"/>
       <c r="D34" s="20" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E34" s="20"/>
       <c r="F34" s="22" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="G34" s="20"/>
       <c r="H34" s="20"/>
@@ -2751,20 +2784,20 @@
       <c r="J34" s="20"/>
     </row>
     <row r="35" spans="1:10" ht="72" x14ac:dyDescent="0.3">
-      <c r="A35" s="28" t="s">
-        <v>106</v>
-      </c>
-      <c r="B35" s="28" t="s">
-        <v>109</v>
-      </c>
-      <c r="C35" s="29" t="s">
+      <c r="A35" s="37" t="s">
+        <v>104</v>
+      </c>
+      <c r="B35" s="37" t="s">
+        <v>107</v>
+      </c>
+      <c r="C35" s="24" t="s">
         <v>56</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>60</v>
+        <v>177</v>
       </c>
       <c r="E35" s="18" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F35" s="18" t="s">
         <v>55</v>
@@ -2775,15 +2808,15 @@
       <c r="J35" s="20"/>
     </row>
     <row r="36" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A36" s="28"/>
-      <c r="B36" s="28"/>
-      <c r="C36" s="29"/>
+      <c r="A36" s="37"/>
+      <c r="B36" s="37"/>
+      <c r="C36" s="24"/>
       <c r="D36" s="18" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E36" s="19"/>
       <c r="F36" s="18" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G36" s="20"/>
       <c r="H36" s="20"/>
@@ -2791,17 +2824,17 @@
       <c r="J36" s="20"/>
     </row>
     <row r="37" spans="1:10" ht="72" x14ac:dyDescent="0.3">
-      <c r="A37" s="28"/>
-      <c r="B37" s="28"/>
-      <c r="C37" s="29"/>
+      <c r="A37" s="37"/>
+      <c r="B37" s="37"/>
+      <c r="C37" s="24"/>
       <c r="D37" s="18" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E37" s="18" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F37" s="18" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G37" s="20"/>
       <c r="H37" s="20"/>
@@ -2809,15 +2842,15 @@
       <c r="J37" s="20"/>
     </row>
     <row r="38" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A38" s="28"/>
-      <c r="B38" s="28"/>
-      <c r="C38" s="29"/>
+      <c r="A38" s="37"/>
+      <c r="B38" s="37"/>
+      <c r="C38" s="24"/>
       <c r="D38" s="22" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E38" s="20"/>
       <c r="F38" s="22" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G38" s="20"/>
       <c r="H38" s="20"/>
@@ -2825,15 +2858,15 @@
       <c r="J38" s="20"/>
     </row>
     <row r="39" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A39" s="28"/>
-      <c r="B39" s="28"/>
-      <c r="C39" s="29"/>
+      <c r="A39" s="37"/>
+      <c r="B39" s="37"/>
+      <c r="C39" s="24"/>
       <c r="D39" s="20" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E39" s="20"/>
       <c r="F39" s="22" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="G39" s="20"/>
       <c r="H39" s="20"/>
@@ -2841,17 +2874,17 @@
       <c r="J39" s="20"/>
     </row>
     <row r="40" spans="1:10" s="1" customFormat="1" ht="60.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="28"/>
-      <c r="B40" s="28"/>
-      <c r="C40" s="32" t="s">
-        <v>95</v>
+      <c r="A40" s="37"/>
+      <c r="B40" s="37"/>
+      <c r="C40" s="25" t="s">
+        <v>93</v>
       </c>
       <c r="D40" s="19" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E40" s="19"/>
       <c r="F40" s="18" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="G40" s="19"/>
       <c r="H40" s="19"/>
@@ -2859,20 +2892,20 @@
       <c r="J40" s="19"/>
     </row>
     <row r="41" spans="1:10" ht="72" x14ac:dyDescent="0.3">
-      <c r="A41" s="28" t="s">
-        <v>108</v>
-      </c>
-      <c r="B41" s="28" t="s">
-        <v>159</v>
-      </c>
-      <c r="C41" s="36" t="s">
+      <c r="A41" s="37" t="s">
+        <v>106</v>
+      </c>
+      <c r="B41" s="37" t="s">
+        <v>156</v>
+      </c>
+      <c r="C41" s="41" t="s">
         <v>56</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>60</v>
+        <v>177</v>
       </c>
       <c r="E41" s="18" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F41" s="18" t="s">
         <v>55</v>
@@ -2883,15 +2916,15 @@
       <c r="J41" s="20"/>
     </row>
     <row r="42" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A42" s="28"/>
-      <c r="B42" s="28"/>
-      <c r="C42" s="36"/>
+      <c r="A42" s="37"/>
+      <c r="B42" s="37"/>
+      <c r="C42" s="41"/>
       <c r="D42" s="18" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E42" s="19"/>
       <c r="F42" s="18" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G42" s="20"/>
       <c r="H42" s="20"/>
@@ -2899,17 +2932,17 @@
       <c r="J42" s="20"/>
     </row>
     <row r="43" spans="1:10" ht="72" x14ac:dyDescent="0.3">
-      <c r="A43" s="28"/>
-      <c r="B43" s="28"/>
-      <c r="C43" s="36"/>
+      <c r="A43" s="37"/>
+      <c r="B43" s="37"/>
+      <c r="C43" s="41"/>
       <c r="D43" s="18" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E43" s="18" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F43" s="18" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G43" s="20"/>
       <c r="H43" s="20"/>
@@ -2917,15 +2950,15 @@
       <c r="J43" s="20"/>
     </row>
     <row r="44" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A44" s="28"/>
-      <c r="B44" s="28"/>
-      <c r="C44" s="36"/>
+      <c r="A44" s="37"/>
+      <c r="B44" s="37"/>
+      <c r="C44" s="41"/>
       <c r="D44" s="22" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E44" s="20"/>
       <c r="F44" s="22" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G44" s="20"/>
       <c r="H44" s="20"/>
@@ -2933,15 +2966,15 @@
       <c r="J44" s="20"/>
     </row>
     <row r="45" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A45" s="28"/>
-      <c r="B45" s="28"/>
-      <c r="C45" s="36"/>
+      <c r="A45" s="37"/>
+      <c r="B45" s="37"/>
+      <c r="C45" s="41"/>
       <c r="D45" s="20" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E45" s="20"/>
       <c r="F45" s="22" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="G45" s="20"/>
       <c r="H45" s="20"/>
@@ -2949,15 +2982,15 @@
       <c r="J45" s="20"/>
     </row>
     <row r="46" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A46" s="28"/>
-      <c r="B46" s="28"/>
-      <c r="C46" s="36"/>
+      <c r="A46" s="37"/>
+      <c r="B46" s="37"/>
+      <c r="C46" s="41"/>
       <c r="D46" s="20" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E46" s="20"/>
       <c r="F46" s="22" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="G46" s="20"/>
       <c r="H46" s="20"/>
@@ -2965,15 +2998,15 @@
       <c r="J46" s="20"/>
     </row>
     <row r="47" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A47" s="28"/>
-      <c r="B47" s="28"/>
-      <c r="C47" s="36"/>
+      <c r="A47" s="37"/>
+      <c r="B47" s="37"/>
+      <c r="C47" s="41"/>
       <c r="D47" s="20" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E47" s="20"/>
       <c r="F47" s="22" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="G47" s="20"/>
       <c r="H47" s="20"/>
@@ -2981,15 +3014,15 @@
       <c r="J47" s="20"/>
     </row>
     <row r="48" spans="1:10" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A48" s="28"/>
-      <c r="B48" s="28"/>
-      <c r="C48" s="36"/>
-      <c r="D48" s="37" t="s">
-        <v>110</v>
+      <c r="A48" s="37"/>
+      <c r="B48" s="37"/>
+      <c r="C48" s="41"/>
+      <c r="D48" s="18" t="s">
+        <v>108</v>
       </c>
       <c r="E48" s="20"/>
       <c r="F48" s="22" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="G48" s="20"/>
       <c r="H48" s="20"/>
@@ -2997,20 +3030,20 @@
       <c r="J48" s="20"/>
     </row>
     <row r="49" spans="1:10" ht="72" x14ac:dyDescent="0.3">
-      <c r="A49" s="28" t="s">
-        <v>112</v>
-      </c>
-      <c r="B49" s="28" t="s">
-        <v>113</v>
-      </c>
-      <c r="C49" s="28" t="s">
+      <c r="A49" s="37" t="s">
+        <v>110</v>
+      </c>
+      <c r="B49" s="37" t="s">
+        <v>181</v>
+      </c>
+      <c r="C49" s="37" t="s">
         <v>56</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>60</v>
+        <v>177</v>
       </c>
       <c r="E49" s="18" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F49" s="18" t="s">
         <v>55</v>
@@ -3021,15 +3054,15 @@
       <c r="J49" s="20"/>
     </row>
     <row r="50" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A50" s="28"/>
-      <c r="B50" s="28"/>
-      <c r="C50" s="28"/>
+      <c r="A50" s="37"/>
+      <c r="B50" s="37"/>
+      <c r="C50" s="37"/>
       <c r="D50" s="18" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E50" s="19"/>
       <c r="F50" s="18" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G50" s="20"/>
       <c r="H50" s="20"/>
@@ -3037,17 +3070,17 @@
       <c r="J50" s="20"/>
     </row>
     <row r="51" spans="1:10" ht="72" x14ac:dyDescent="0.3">
-      <c r="A51" s="28"/>
-      <c r="B51" s="28"/>
-      <c r="C51" s="28"/>
+      <c r="A51" s="37"/>
+      <c r="B51" s="37"/>
+      <c r="C51" s="37"/>
       <c r="D51" s="18" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E51" s="18" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F51" s="18" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G51" s="20"/>
       <c r="H51" s="20"/>
@@ -3055,15 +3088,15 @@
       <c r="J51" s="20"/>
     </row>
     <row r="52" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A52" s="28"/>
-      <c r="B52" s="28"/>
-      <c r="C52" s="28"/>
+      <c r="A52" s="37"/>
+      <c r="B52" s="37"/>
+      <c r="C52" s="37"/>
       <c r="D52" s="22" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E52" s="20"/>
       <c r="F52" s="22" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G52" s="20"/>
       <c r="H52" s="20"/>
@@ -3071,15 +3104,15 @@
       <c r="J52" s="20"/>
     </row>
     <row r="53" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A53" s="28"/>
-      <c r="B53" s="28"/>
-      <c r="C53" s="28"/>
+      <c r="A53" s="37"/>
+      <c r="B53" s="37"/>
+      <c r="C53" s="37"/>
       <c r="D53" s="20" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E53" s="20"/>
       <c r="F53" s="22" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="G53" s="20"/>
       <c r="H53" s="20"/>
@@ -3087,15 +3120,15 @@
       <c r="J53" s="20"/>
     </row>
     <row r="54" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A54" s="28"/>
-      <c r="B54" s="28"/>
-      <c r="C54" s="28"/>
+      <c r="A54" s="37"/>
+      <c r="B54" s="37"/>
+      <c r="C54" s="37"/>
       <c r="D54" s="20" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E54" s="20"/>
       <c r="F54" s="22" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="G54" s="20"/>
       <c r="H54" s="20"/>
@@ -3103,15 +3136,15 @@
       <c r="J54" s="20"/>
     </row>
     <row r="55" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A55" s="28"/>
-      <c r="B55" s="28"/>
-      <c r="C55" s="28"/>
+      <c r="A55" s="37"/>
+      <c r="B55" s="37"/>
+      <c r="C55" s="37"/>
       <c r="D55" s="20" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E55" s="20"/>
       <c r="F55" s="22" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="G55" s="20"/>
       <c r="H55" s="20"/>
@@ -3119,17 +3152,17 @@
       <c r="J55" s="20"/>
     </row>
     <row r="56" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A56" s="28"/>
-      <c r="B56" s="28"/>
-      <c r="C56" s="28"/>
+      <c r="A56" s="37"/>
+      <c r="B56" s="37"/>
+      <c r="C56" s="37"/>
       <c r="D56" s="22" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="E56" s="21" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="F56" s="22" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="G56" s="20"/>
       <c r="H56" s="20"/>
@@ -3137,15 +3170,15 @@
       <c r="J56" s="20"/>
     </row>
     <row r="57" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A57" s="28"/>
-      <c r="B57" s="28"/>
-      <c r="C57" s="28"/>
+      <c r="A57" s="37"/>
+      <c r="B57" s="37"/>
+      <c r="C57" s="37"/>
       <c r="D57" s="20" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E57" s="20"/>
       <c r="F57" s="22" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="G57" s="20"/>
       <c r="H57" s="20"/>
@@ -3153,20 +3186,20 @@
       <c r="J57" s="20"/>
     </row>
     <row r="58" spans="1:10" ht="72" x14ac:dyDescent="0.3">
-      <c r="A58" s="25" t="s">
-        <v>119</v>
-      </c>
-      <c r="B58" s="25" t="s">
-        <v>120</v>
-      </c>
-      <c r="C58" s="28" t="s">
+      <c r="A58" s="38" t="s">
+        <v>116</v>
+      </c>
+      <c r="B58" s="38" t="s">
+        <v>117</v>
+      </c>
+      <c r="C58" s="37" t="s">
         <v>56</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>60</v>
+        <v>177</v>
       </c>
       <c r="E58" s="18" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F58" s="18" t="s">
         <v>55</v>
@@ -3177,15 +3210,15 @@
       <c r="J58" s="20"/>
     </row>
     <row r="59" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A59" s="26"/>
-      <c r="B59" s="26"/>
-      <c r="C59" s="28"/>
+      <c r="A59" s="39"/>
+      <c r="B59" s="39"/>
+      <c r="C59" s="37"/>
       <c r="D59" s="18" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E59" s="19"/>
       <c r="F59" s="18" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G59" s="20"/>
       <c r="H59" s="20"/>
@@ -3193,17 +3226,17 @@
       <c r="J59" s="20"/>
     </row>
     <row r="60" spans="1:10" ht="72" x14ac:dyDescent="0.3">
-      <c r="A60" s="26"/>
-      <c r="B60" s="26"/>
-      <c r="C60" s="28"/>
+      <c r="A60" s="39"/>
+      <c r="B60" s="39"/>
+      <c r="C60" s="37"/>
       <c r="D60" s="18" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E60" s="18" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F60" s="18" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G60" s="20"/>
       <c r="H60" s="20"/>
@@ -3211,15 +3244,15 @@
       <c r="J60" s="20"/>
     </row>
     <row r="61" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A61" s="26"/>
-      <c r="B61" s="26"/>
-      <c r="C61" s="28"/>
+      <c r="A61" s="39"/>
+      <c r="B61" s="39"/>
+      <c r="C61" s="37"/>
       <c r="D61" s="22" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E61" s="20"/>
       <c r="F61" s="22" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G61" s="20"/>
       <c r="H61" s="20"/>
@@ -3227,15 +3260,15 @@
       <c r="J61" s="20"/>
     </row>
     <row r="62" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A62" s="26"/>
-      <c r="B62" s="26"/>
-      <c r="C62" s="28"/>
+      <c r="A62" s="39"/>
+      <c r="B62" s="39"/>
+      <c r="C62" s="37"/>
       <c r="D62" s="20" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E62" s="20"/>
       <c r="F62" s="22" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="G62" s="20"/>
       <c r="H62" s="20"/>
@@ -3243,15 +3276,15 @@
       <c r="J62" s="20"/>
     </row>
     <row r="63" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A63" s="26"/>
-      <c r="B63" s="26"/>
-      <c r="C63" s="28"/>
+      <c r="A63" s="39"/>
+      <c r="B63" s="39"/>
+      <c r="C63" s="37"/>
       <c r="D63" s="20" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E63" s="20"/>
       <c r="F63" s="22" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="G63" s="20"/>
       <c r="H63" s="20"/>
@@ -3259,15 +3292,15 @@
       <c r="J63" s="20"/>
     </row>
     <row r="64" spans="1:10" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A64" s="26"/>
-      <c r="B64" s="26"/>
+      <c r="A64" s="39"/>
+      <c r="B64" s="39"/>
       <c r="C64" s="19"/>
       <c r="D64" s="19" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E64" s="19"/>
       <c r="F64" s="18" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="G64" s="19"/>
       <c r="H64" s="19"/>
@@ -3275,19 +3308,19 @@
       <c r="J64" s="19"/>
     </row>
     <row r="65" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A65" s="27"/>
-      <c r="B65" s="27"/>
-      <c r="C65" s="32" t="s">
-        <v>95</v>
+      <c r="A65" s="40"/>
+      <c r="B65" s="40"/>
+      <c r="C65" s="25" t="s">
+        <v>93</v>
       </c>
       <c r="D65" s="18" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="E65" s="18" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="F65" s="22" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="G65" s="20"/>
       <c r="H65" s="20"/>
@@ -3295,20 +3328,20 @@
       <c r="J65" s="20"/>
     </row>
     <row r="66" spans="1:10" ht="72" x14ac:dyDescent="0.3">
-      <c r="A66" s="25" t="s">
-        <v>124</v>
-      </c>
-      <c r="B66" s="25" t="s">
-        <v>125</v>
-      </c>
-      <c r="C66" s="28" t="s">
+      <c r="A66" s="38" t="s">
+        <v>121</v>
+      </c>
+      <c r="B66" s="38" t="s">
+        <v>122</v>
+      </c>
+      <c r="C66" s="37" t="s">
         <v>56</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>60</v>
+        <v>177</v>
       </c>
       <c r="E66" s="18" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F66" s="18" t="s">
         <v>55</v>
@@ -3319,15 +3352,15 @@
       <c r="J66" s="20"/>
     </row>
     <row r="67" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A67" s="26"/>
-      <c r="B67" s="26"/>
-      <c r="C67" s="28"/>
+      <c r="A67" s="39"/>
+      <c r="B67" s="39"/>
+      <c r="C67" s="37"/>
       <c r="D67" s="18" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E67" s="19"/>
       <c r="F67" s="18" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G67" s="20"/>
       <c r="H67" s="20"/>
@@ -3335,17 +3368,17 @@
       <c r="J67" s="20"/>
     </row>
     <row r="68" spans="1:10" ht="72" x14ac:dyDescent="0.3">
-      <c r="A68" s="26"/>
-      <c r="B68" s="26"/>
-      <c r="C68" s="28"/>
+      <c r="A68" s="39"/>
+      <c r="B68" s="39"/>
+      <c r="C68" s="37"/>
       <c r="D68" s="18" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E68" s="18" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F68" s="18" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G68" s="20"/>
       <c r="H68" s="20"/>
@@ -3353,15 +3386,15 @@
       <c r="J68" s="20"/>
     </row>
     <row r="69" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A69" s="26"/>
-      <c r="B69" s="26"/>
-      <c r="C69" s="28"/>
+      <c r="A69" s="39"/>
+      <c r="B69" s="39"/>
+      <c r="C69" s="37"/>
       <c r="D69" s="22" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E69" s="20"/>
       <c r="F69" s="22" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G69" s="20"/>
       <c r="H69" s="20"/>
@@ -3369,15 +3402,15 @@
       <c r="J69" s="20"/>
     </row>
     <row r="70" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A70" s="26"/>
-      <c r="B70" s="26"/>
-      <c r="C70" s="28"/>
+      <c r="A70" s="39"/>
+      <c r="B70" s="39"/>
+      <c r="C70" s="37"/>
       <c r="D70" s="20" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E70" s="20"/>
       <c r="F70" s="22" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="G70" s="20"/>
       <c r="H70" s="20"/>
@@ -3385,15 +3418,15 @@
       <c r="J70" s="20"/>
     </row>
     <row r="71" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A71" s="26"/>
-      <c r="B71" s="26"/>
-      <c r="C71" s="28"/>
+      <c r="A71" s="39"/>
+      <c r="B71" s="39"/>
+      <c r="C71" s="37"/>
       <c r="D71" s="20" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E71" s="20"/>
       <c r="F71" s="22" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="G71" s="20"/>
       <c r="H71" s="20"/>
@@ -3401,15 +3434,15 @@
       <c r="J71" s="20"/>
     </row>
     <row r="72" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A72" s="26"/>
-      <c r="B72" s="26"/>
+      <c r="A72" s="39"/>
+      <c r="B72" s="39"/>
       <c r="C72" s="19"/>
       <c r="D72" s="19" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E72" s="19"/>
       <c r="F72" s="18" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="G72" s="20"/>
       <c r="H72" s="20"/>
@@ -3417,19 +3450,19 @@
       <c r="J72" s="20"/>
     </row>
     <row r="73" spans="1:10" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A73" s="27"/>
-      <c r="B73" s="27"/>
-      <c r="C73" s="32" t="s">
-        <v>95</v>
+      <c r="A73" s="40"/>
+      <c r="B73" s="40"/>
+      <c r="C73" s="25" t="s">
+        <v>93</v>
       </c>
       <c r="D73" s="18" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="E73" s="18" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="F73" s="18" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="G73" s="20"/>
       <c r="H73" s="20"/>
@@ -3437,20 +3470,20 @@
       <c r="J73" s="20"/>
     </row>
     <row r="74" spans="1:10" ht="72" x14ac:dyDescent="0.3">
-      <c r="A74" s="28" t="s">
-        <v>129</v>
-      </c>
-      <c r="B74" s="28" t="s">
-        <v>130</v>
-      </c>
-      <c r="C74" s="29" t="s">
+      <c r="A74" s="37" t="s">
+        <v>126</v>
+      </c>
+      <c r="B74" s="37" t="s">
+        <v>127</v>
+      </c>
+      <c r="C74" s="24" t="s">
         <v>56</v>
       </c>
       <c r="D74" s="2" t="s">
-        <v>60</v>
+        <v>177</v>
       </c>
       <c r="E74" s="18" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F74" s="18" t="s">
         <v>55</v>
@@ -3461,15 +3494,15 @@
       <c r="J74" s="20"/>
     </row>
     <row r="75" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A75" s="28"/>
-      <c r="B75" s="28"/>
-      <c r="C75" s="29"/>
+      <c r="A75" s="37"/>
+      <c r="B75" s="37"/>
+      <c r="C75" s="24"/>
       <c r="D75" s="18" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E75" s="19"/>
       <c r="F75" s="18" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G75" s="20"/>
       <c r="H75" s="20"/>
@@ -3477,17 +3510,17 @@
       <c r="J75" s="20"/>
     </row>
     <row r="76" spans="1:10" ht="72" x14ac:dyDescent="0.3">
-      <c r="A76" s="28"/>
-      <c r="B76" s="28"/>
-      <c r="C76" s="29"/>
+      <c r="A76" s="37"/>
+      <c r="B76" s="37"/>
+      <c r="C76" s="24"/>
       <c r="D76" s="18" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E76" s="18" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F76" s="18" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G76" s="20"/>
       <c r="H76" s="20"/>
@@ -3495,15 +3528,15 @@
       <c r="J76" s="20"/>
     </row>
     <row r="77" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A77" s="28"/>
-      <c r="B77" s="28"/>
-      <c r="C77" s="29"/>
+      <c r="A77" s="37"/>
+      <c r="B77" s="37"/>
+      <c r="C77" s="24"/>
       <c r="D77" s="22" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E77" s="20"/>
       <c r="F77" s="22" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G77" s="20"/>
       <c r="H77" s="20"/>
@@ -3511,15 +3544,15 @@
       <c r="J77" s="20"/>
     </row>
     <row r="78" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A78" s="28"/>
-      <c r="B78" s="28"/>
-      <c r="C78" s="29"/>
+      <c r="A78" s="37"/>
+      <c r="B78" s="37"/>
+      <c r="C78" s="24"/>
       <c r="D78" s="20" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E78" s="20"/>
       <c r="F78" s="22" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="G78" s="20"/>
       <c r="H78" s="20"/>
@@ -3527,17 +3560,17 @@
       <c r="J78" s="20"/>
     </row>
     <row r="79" spans="1:10" s="1" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A79" s="28"/>
-      <c r="B79" s="28"/>
-      <c r="C79" s="32" t="s">
-        <v>131</v>
+      <c r="A79" s="37"/>
+      <c r="B79" s="37"/>
+      <c r="C79" s="25" t="s">
+        <v>128</v>
       </c>
       <c r="D79" s="19" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E79" s="19"/>
       <c r="F79" s="18" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="G79" s="19"/>
       <c r="H79" s="19"/>
@@ -3545,30 +3578,130 @@
       <c r="J79" s="19"/>
     </row>
     <row r="80" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A80" s="28"/>
-      <c r="B80" s="28"/>
+      <c r="A80" s="37"/>
+      <c r="B80" s="37"/>
       <c r="C80" s="19"/>
       <c r="D80" s="19" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E80" s="19"/>
       <c r="F80" s="18" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="G80" s="20"/>
       <c r="H80" s="20"/>
       <c r="I80" s="20"/>
       <c r="J80" s="20"/>
     </row>
-    <row r="81" spans="1:6" s="31" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A81" s="30"/>
-      <c r="B81" s="30"/>
-      <c r="D81" s="38"/>
-      <c r="E81" s="38"/>
-      <c r="F81" s="38"/>
+    <row r="81" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+      <c r="A81" s="37" t="s">
+        <v>178</v>
+      </c>
+      <c r="B81" s="37" t="s">
+        <v>179</v>
+      </c>
+      <c r="C81" s="37" t="s">
+        <v>56</v>
+      </c>
+      <c r="D81" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="E81" s="18" t="s">
+        <v>61</v>
+      </c>
+      <c r="F81" s="18" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A82" s="37"/>
+      <c r="B82" s="37"/>
+      <c r="C82" s="37"/>
+      <c r="D82" s="18" t="s">
+        <v>65</v>
+      </c>
+      <c r="E82" s="19"/>
+      <c r="F82" s="18" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+      <c r="A83" s="37"/>
+      <c r="B83" s="37"/>
+      <c r="C83" s="37"/>
+      <c r="D83" s="18" t="s">
+        <v>71</v>
+      </c>
+      <c r="E83" s="18" t="s">
+        <v>70</v>
+      </c>
+      <c r="F83" s="18" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A84" s="37"/>
+      <c r="B84" s="37"/>
+      <c r="C84" s="37"/>
+      <c r="D84" s="22" t="s">
+        <v>68</v>
+      </c>
+      <c r="E84" s="20"/>
+      <c r="F84" s="22" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A85" s="37"/>
+      <c r="B85" s="37"/>
+      <c r="C85" s="37"/>
+      <c r="D85" s="20" t="s">
+        <v>81</v>
+      </c>
+      <c r="E85" s="20"/>
+      <c r="F85" s="22" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A86" s="37"/>
+      <c r="B86" s="37"/>
+      <c r="C86" s="37"/>
+      <c r="D86" s="20" t="s">
+        <v>83</v>
+      </c>
+      <c r="E86" s="20"/>
+      <c r="F86" s="22" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A87" s="37"/>
+      <c r="B87" s="37"/>
+      <c r="C87" s="25" t="s">
+        <v>93</v>
+      </c>
+      <c r="D87" s="22" t="s">
+        <v>188</v>
+      </c>
+      <c r="E87" s="20"/>
+      <c r="F87" s="22" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A88" s="37"/>
+      <c r="B88" s="37"/>
+      <c r="C88" s="24"/>
+      <c r="D88" s="20"/>
+      <c r="E88" s="20"/>
+      <c r="F88" s="22"/>
     </row>
   </sheetData>
-  <mergeCells count="28">
+  <mergeCells count="31">
+    <mergeCell ref="C81:C86"/>
+    <mergeCell ref="A81:A88"/>
+    <mergeCell ref="B81:B88"/>
     <mergeCell ref="B74:B80"/>
     <mergeCell ref="A74:A80"/>
     <mergeCell ref="C58:C63"/>
@@ -3588,15 +3721,15 @@
     <mergeCell ref="A19:A25"/>
     <mergeCell ref="A26:A34"/>
     <mergeCell ref="B26:B34"/>
+    <mergeCell ref="C2:C10"/>
+    <mergeCell ref="B2:B10"/>
+    <mergeCell ref="A2:A10"/>
     <mergeCell ref="C26:C34"/>
     <mergeCell ref="C11:C16"/>
     <mergeCell ref="A11:A18"/>
     <mergeCell ref="B11:B18"/>
     <mergeCell ref="C19:C24"/>
     <mergeCell ref="B19:B25"/>
-    <mergeCell ref="C2:C10"/>
-    <mergeCell ref="B2:B10"/>
-    <mergeCell ref="A2:A10"/>
   </mergeCells>
   <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3605,10 +3738,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A6BF4CD-E2F7-49FC-B635-1E7D396807B0}">
-  <dimension ref="A1:J73"/>
+  <dimension ref="A1:J81"/>
   <sheetViews>
-    <sheetView topLeftCell="A66" workbookViewId="0">
-      <selection activeCell="C66" sqref="C66:C71"/>
+    <sheetView topLeftCell="A74" workbookViewId="0">
+      <selection activeCell="F81" sqref="C74:F81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3659,20 +3792,20 @@
       </c>
     </row>
     <row r="2" spans="1:10" s="1" customFormat="1" ht="125.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="28" t="s">
+      <c r="A2" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="28" t="s">
-        <v>133</v>
-      </c>
-      <c r="C2" s="28" t="s">
+      <c r="B2" s="37" t="s">
+        <v>130</v>
+      </c>
+      <c r="C2" s="37" t="s">
         <v>56</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>60</v>
+        <v>177</v>
       </c>
       <c r="E2" s="18" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F2" s="18" t="s">
         <v>55</v>
@@ -3683,15 +3816,15 @@
       <c r="J2" s="2"/>
     </row>
     <row r="3" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A3" s="28"/>
-      <c r="B3" s="28"/>
-      <c r="C3" s="28"/>
+      <c r="A3" s="37"/>
+      <c r="B3" s="37"/>
+      <c r="C3" s="37"/>
       <c r="D3" s="18" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E3" s="19"/>
       <c r="F3" s="18" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G3" s="19"/>
       <c r="H3" s="19"/>
@@ -3699,17 +3832,17 @@
       <c r="J3" s="19"/>
     </row>
     <row r="4" spans="1:10" ht="72" x14ac:dyDescent="0.3">
-      <c r="A4" s="28"/>
-      <c r="B4" s="28"/>
-      <c r="C4" s="28"/>
+      <c r="A4" s="37"/>
+      <c r="B4" s="37"/>
+      <c r="C4" s="37"/>
       <c r="D4" s="18" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E4" s="18" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F4" s="18" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G4" s="20"/>
       <c r="H4" s="20"/>
@@ -3717,15 +3850,15 @@
       <c r="J4" s="20"/>
     </row>
     <row r="5" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A5" s="28"/>
-      <c r="B5" s="28"/>
-      <c r="C5" s="28"/>
+      <c r="A5" s="37"/>
+      <c r="B5" s="37"/>
+      <c r="C5" s="37"/>
       <c r="D5" s="22" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E5" s="20"/>
       <c r="F5" s="22" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G5" s="20"/>
       <c r="H5" s="20"/>
@@ -3733,15 +3866,15 @@
       <c r="J5" s="20"/>
     </row>
     <row r="6" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A6" s="28"/>
-      <c r="B6" s="28"/>
-      <c r="C6" s="28"/>
+      <c r="A6" s="37"/>
+      <c r="B6" s="37"/>
+      <c r="C6" s="37"/>
       <c r="D6" s="20" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E6" s="20"/>
       <c r="F6" s="22" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="G6" s="20"/>
       <c r="H6" s="20"/>
@@ -3749,15 +3882,15 @@
       <c r="J6" s="20"/>
     </row>
     <row r="7" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A7" s="28"/>
-      <c r="B7" s="28"/>
-      <c r="C7" s="28"/>
+      <c r="A7" s="37"/>
+      <c r="B7" s="37"/>
+      <c r="C7" s="37"/>
       <c r="D7" s="20" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="E7" s="20"/>
       <c r="F7" s="22" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="G7" s="20"/>
       <c r="H7" s="20"/>
@@ -3765,15 +3898,15 @@
       <c r="J7" s="20"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A8" s="28"/>
-      <c r="B8" s="28"/>
-      <c r="C8" s="28"/>
+      <c r="A8" s="37"/>
+      <c r="B8" s="37"/>
+      <c r="C8" s="37"/>
       <c r="D8" s="20" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E8" s="20"/>
       <c r="F8" s="22" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="G8" s="20"/>
       <c r="H8" s="20"/>
@@ -3781,17 +3914,17 @@
       <c r="J8" s="20"/>
     </row>
     <row r="9" spans="1:10" ht="46.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="28"/>
-      <c r="B9" s="28"/>
-      <c r="C9" s="28"/>
+      <c r="A9" s="37"/>
+      <c r="B9" s="37"/>
+      <c r="C9" s="37"/>
       <c r="D9" s="18" t="s">
-        <v>135</v>
-      </c>
-      <c r="E9" s="35" t="s">
-        <v>139</v>
+        <v>132</v>
+      </c>
+      <c r="E9" s="28" t="s">
+        <v>136</v>
       </c>
       <c r="F9" s="22" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="G9" s="20"/>
       <c r="H9" s="20"/>
@@ -3799,15 +3932,15 @@
       <c r="J9" s="20"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A10" s="28"/>
-      <c r="B10" s="28"/>
-      <c r="C10" s="28"/>
+      <c r="A10" s="37"/>
+      <c r="B10" s="37"/>
+      <c r="C10" s="37"/>
       <c r="D10" s="20" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E10" s="20"/>
       <c r="F10" s="22" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="G10" s="20"/>
       <c r="H10" s="20"/>
@@ -3815,20 +3948,20 @@
       <c r="J10" s="20"/>
     </row>
     <row r="11" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="28" t="s">
+      <c r="A11" s="37" t="s">
         <v>52</v>
       </c>
-      <c r="B11" s="28" t="s">
-        <v>138</v>
-      </c>
-      <c r="C11" s="28" t="s">
+      <c r="B11" s="37" t="s">
+        <v>135</v>
+      </c>
+      <c r="C11" s="37" t="s">
         <v>56</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>60</v>
+        <v>177</v>
       </c>
       <c r="E11" s="18" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F11" s="18" t="s">
         <v>55</v>
@@ -3839,15 +3972,15 @@
       <c r="J11" s="20"/>
     </row>
     <row r="12" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A12" s="28"/>
-      <c r="B12" s="28"/>
-      <c r="C12" s="28"/>
+      <c r="A12" s="37"/>
+      <c r="B12" s="37"/>
+      <c r="C12" s="37"/>
       <c r="D12" s="18" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E12" s="19"/>
       <c r="F12" s="18" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G12" s="20"/>
       <c r="H12" s="20"/>
@@ -3855,17 +3988,17 @@
       <c r="J12" s="20"/>
     </row>
     <row r="13" spans="1:10" ht="72" x14ac:dyDescent="0.3">
-      <c r="A13" s="28"/>
-      <c r="B13" s="28"/>
-      <c r="C13" s="28"/>
+      <c r="A13" s="37"/>
+      <c r="B13" s="37"/>
+      <c r="C13" s="37"/>
       <c r="D13" s="18" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E13" s="18" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F13" s="18" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G13" s="20"/>
       <c r="H13" s="20"/>
@@ -3873,15 +4006,15 @@
       <c r="J13" s="20"/>
     </row>
     <row r="14" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A14" s="28"/>
-      <c r="B14" s="28"/>
-      <c r="C14" s="28"/>
+      <c r="A14" s="37"/>
+      <c r="B14" s="37"/>
+      <c r="C14" s="37"/>
       <c r="D14" s="22" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E14" s="20"/>
       <c r="F14" s="22" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G14" s="20"/>
       <c r="H14" s="20"/>
@@ -3889,15 +4022,15 @@
       <c r="J14" s="20"/>
     </row>
     <row r="15" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A15" s="28"/>
-      <c r="B15" s="28"/>
-      <c r="C15" s="28"/>
+      <c r="A15" s="37"/>
+      <c r="B15" s="37"/>
+      <c r="C15" s="37"/>
       <c r="D15" s="20" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E15" s="20"/>
       <c r="F15" s="22" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="G15" s="20"/>
       <c r="H15" s="20"/>
@@ -3905,15 +4038,15 @@
       <c r="J15" s="20"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A16" s="28"/>
-      <c r="B16" s="28"/>
-      <c r="C16" s="28"/>
+      <c r="A16" s="37"/>
+      <c r="B16" s="37"/>
+      <c r="C16" s="37"/>
       <c r="D16" s="20" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="E16" s="20"/>
       <c r="F16" s="22" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="G16" s="20"/>
       <c r="H16" s="20"/>
@@ -3921,17 +4054,17 @@
       <c r="J16" s="20"/>
     </row>
     <row r="17" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A17" s="28"/>
-      <c r="B17" s="28"/>
-      <c r="C17" s="32" t="s">
-        <v>141</v>
+      <c r="A17" s="37"/>
+      <c r="B17" s="37"/>
+      <c r="C17" s="25" t="s">
+        <v>138</v>
       </c>
       <c r="D17" s="19" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="E17" s="20"/>
       <c r="F17" s="18" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="G17" s="20"/>
       <c r="H17" s="20"/>
@@ -3939,17 +4072,17 @@
       <c r="J17" s="20"/>
     </row>
     <row r="18" spans="1:10" s="1" customFormat="1" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A18" s="28"/>
-      <c r="B18" s="28"/>
-      <c r="C18" s="32"/>
+      <c r="A18" s="37"/>
+      <c r="B18" s="37"/>
+      <c r="C18" s="25"/>
       <c r="D18" s="19" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="E18" s="18" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="F18" s="18" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="G18" s="19"/>
       <c r="H18" s="19"/>
@@ -3957,20 +4090,20 @@
       <c r="J18" s="19"/>
     </row>
     <row r="19" spans="1:10" ht="72" x14ac:dyDescent="0.3">
-      <c r="A19" s="28" t="s">
-        <v>73</v>
-      </c>
-      <c r="B19" s="28" t="s">
-        <v>147</v>
-      </c>
-      <c r="C19" s="28" t="s">
+      <c r="A19" s="37" t="s">
+        <v>72</v>
+      </c>
+      <c r="B19" s="37" t="s">
+        <v>144</v>
+      </c>
+      <c r="C19" s="37" t="s">
         <v>56</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>60</v>
+        <v>177</v>
       </c>
       <c r="E19" s="18" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F19" s="18" t="s">
         <v>55</v>
@@ -3981,15 +4114,15 @@
       <c r="J19" s="20"/>
     </row>
     <row r="20" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A20" s="28"/>
-      <c r="B20" s="28"/>
-      <c r="C20" s="28"/>
+      <c r="A20" s="37"/>
+      <c r="B20" s="37"/>
+      <c r="C20" s="37"/>
       <c r="D20" s="18" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E20" s="19"/>
       <c r="F20" s="18" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G20" s="20"/>
       <c r="H20" s="20"/>
@@ -3997,17 +4130,17 @@
       <c r="J20" s="20"/>
     </row>
     <row r="21" spans="1:10" ht="72" x14ac:dyDescent="0.3">
-      <c r="A21" s="28"/>
-      <c r="B21" s="28"/>
-      <c r="C21" s="28"/>
+      <c r="A21" s="37"/>
+      <c r="B21" s="37"/>
+      <c r="C21" s="37"/>
       <c r="D21" s="18" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E21" s="18" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F21" s="18" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G21" s="20"/>
       <c r="H21" s="20"/>
@@ -4015,15 +4148,15 @@
       <c r="J21" s="20"/>
     </row>
     <row r="22" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A22" s="28"/>
-      <c r="B22" s="28"/>
-      <c r="C22" s="28"/>
+      <c r="A22" s="37"/>
+      <c r="B22" s="37"/>
+      <c r="C22" s="37"/>
       <c r="D22" s="22" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E22" s="20"/>
       <c r="F22" s="22" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G22" s="20"/>
       <c r="H22" s="20"/>
@@ -4031,15 +4164,15 @@
       <c r="J22" s="20"/>
     </row>
     <row r="23" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A23" s="28"/>
-      <c r="B23" s="28"/>
-      <c r="C23" s="28"/>
+      <c r="A23" s="37"/>
+      <c r="B23" s="37"/>
+      <c r="C23" s="37"/>
       <c r="D23" s="20" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E23" s="20"/>
       <c r="F23" s="22" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="G23" s="20"/>
       <c r="H23" s="20"/>
@@ -4047,15 +4180,15 @@
       <c r="J23" s="20"/>
     </row>
     <row r="24" spans="1:10" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="28"/>
-      <c r="B24" s="28"/>
-      <c r="C24" s="28"/>
+      <c r="A24" s="37"/>
+      <c r="B24" s="37"/>
+      <c r="C24" s="37"/>
       <c r="D24" s="20" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="E24" s="20"/>
       <c r="F24" s="22" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="G24" s="20"/>
       <c r="H24" s="20"/>
@@ -4063,19 +4196,19 @@
       <c r="J24" s="20"/>
     </row>
     <row r="25" spans="1:10" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="28"/>
-      <c r="B25" s="28"/>
+      <c r="A25" s="37"/>
+      <c r="B25" s="37"/>
       <c r="C25" s="23" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D25" s="19" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="E25" s="18" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="F25" s="18" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="G25" s="20"/>
       <c r="H25" s="20"/>
@@ -4083,20 +4216,20 @@
       <c r="J25" s="20"/>
     </row>
     <row r="26" spans="1:10" ht="72" x14ac:dyDescent="0.3">
-      <c r="A26" s="28" t="s">
-        <v>78</v>
-      </c>
-      <c r="B26" s="28" t="s">
-        <v>151</v>
-      </c>
-      <c r="C26" s="28" t="s">
+      <c r="A26" s="37" t="s">
+        <v>76</v>
+      </c>
+      <c r="B26" s="37" t="s">
+        <v>148</v>
+      </c>
+      <c r="C26" s="37" t="s">
         <v>56</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>60</v>
+        <v>177</v>
       </c>
       <c r="E26" s="18" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F26" s="18" t="s">
         <v>55</v>
@@ -4107,15 +4240,15 @@
       <c r="J26" s="20"/>
     </row>
     <row r="27" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A27" s="28"/>
-      <c r="B27" s="28"/>
-      <c r="C27" s="28"/>
+      <c r="A27" s="37"/>
+      <c r="B27" s="37"/>
+      <c r="C27" s="37"/>
       <c r="D27" s="18" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E27" s="19"/>
       <c r="F27" s="18" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G27" s="20"/>
       <c r="H27" s="20"/>
@@ -4123,17 +4256,17 @@
       <c r="J27" s="20"/>
     </row>
     <row r="28" spans="1:10" ht="72" x14ac:dyDescent="0.3">
-      <c r="A28" s="28"/>
-      <c r="B28" s="28"/>
-      <c r="C28" s="28"/>
+      <c r="A28" s="37"/>
+      <c r="B28" s="37"/>
+      <c r="C28" s="37"/>
       <c r="D28" s="18" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E28" s="18" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F28" s="18" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G28" s="20"/>
       <c r="H28" s="20"/>
@@ -4141,15 +4274,15 @@
       <c r="J28" s="20"/>
     </row>
     <row r="29" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A29" s="28"/>
-      <c r="B29" s="28"/>
-      <c r="C29" s="28"/>
+      <c r="A29" s="37"/>
+      <c r="B29" s="37"/>
+      <c r="C29" s="37"/>
       <c r="D29" s="22" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E29" s="20"/>
       <c r="F29" s="22" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G29" s="20"/>
       <c r="H29" s="20"/>
@@ -4157,15 +4290,15 @@
       <c r="J29" s="20"/>
     </row>
     <row r="30" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A30" s="28"/>
-      <c r="B30" s="28"/>
-      <c r="C30" s="28"/>
+      <c r="A30" s="37"/>
+      <c r="B30" s="37"/>
+      <c r="C30" s="37"/>
       <c r="D30" s="20" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E30" s="20"/>
       <c r="F30" s="22" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="G30" s="20"/>
       <c r="H30" s="20"/>
@@ -4173,15 +4306,15 @@
       <c r="J30" s="20"/>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A31" s="28"/>
-      <c r="B31" s="28"/>
-      <c r="C31" s="28"/>
+      <c r="A31" s="37"/>
+      <c r="B31" s="37"/>
+      <c r="C31" s="37"/>
       <c r="D31" s="20" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="E31" s="20"/>
       <c r="F31" s="22" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="G31" s="20"/>
       <c r="H31" s="20"/>
@@ -4189,15 +4322,15 @@
       <c r="J31" s="20"/>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A32" s="28"/>
-      <c r="B32" s="28"/>
-      <c r="C32" s="28"/>
+      <c r="A32" s="37"/>
+      <c r="B32" s="37"/>
+      <c r="C32" s="37"/>
       <c r="D32" s="20" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E32" s="20"/>
       <c r="F32" s="22" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="G32" s="20"/>
       <c r="H32" s="20"/>
@@ -4205,17 +4338,17 @@
       <c r="J32" s="20"/>
     </row>
     <row r="33" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A33" s="28"/>
-      <c r="B33" s="28"/>
-      <c r="C33" s="28"/>
+      <c r="A33" s="37"/>
+      <c r="B33" s="37"/>
+      <c r="C33" s="37"/>
       <c r="D33" s="22" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="E33" s="21" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="F33" s="22" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="G33" s="20"/>
       <c r="H33" s="20"/>
@@ -4223,15 +4356,15 @@
       <c r="J33" s="20"/>
     </row>
     <row r="34" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A34" s="28"/>
-      <c r="B34" s="28"/>
-      <c r="C34" s="28"/>
+      <c r="A34" s="37"/>
+      <c r="B34" s="37"/>
+      <c r="C34" s="37"/>
       <c r="D34" s="20" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E34" s="20"/>
       <c r="F34" s="22" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="G34" s="20"/>
       <c r="H34" s="20"/>
@@ -4239,20 +4372,20 @@
       <c r="J34" s="20"/>
     </row>
     <row r="35" spans="1:10" ht="72" x14ac:dyDescent="0.3">
-      <c r="A35" s="28" t="s">
-        <v>106</v>
-      </c>
-      <c r="B35" s="28" t="s">
-        <v>155</v>
-      </c>
-      <c r="C35" s="29" t="s">
+      <c r="A35" s="37" t="s">
+        <v>104</v>
+      </c>
+      <c r="B35" s="37" t="s">
+        <v>152</v>
+      </c>
+      <c r="C35" s="24" t="s">
         <v>56</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>60</v>
+        <v>177</v>
       </c>
       <c r="E35" s="18" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F35" s="18" t="s">
         <v>55</v>
@@ -4263,15 +4396,15 @@
       <c r="J35" s="20"/>
     </row>
     <row r="36" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A36" s="28"/>
-      <c r="B36" s="28"/>
-      <c r="C36" s="29"/>
+      <c r="A36" s="37"/>
+      <c r="B36" s="37"/>
+      <c r="C36" s="24"/>
       <c r="D36" s="18" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E36" s="19"/>
       <c r="F36" s="18" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G36" s="20"/>
       <c r="H36" s="20"/>
@@ -4279,17 +4412,17 @@
       <c r="J36" s="20"/>
     </row>
     <row r="37" spans="1:10" ht="72" x14ac:dyDescent="0.3">
-      <c r="A37" s="28"/>
-      <c r="B37" s="28"/>
-      <c r="C37" s="29"/>
+      <c r="A37" s="37"/>
+      <c r="B37" s="37"/>
+      <c r="C37" s="24"/>
       <c r="D37" s="18" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E37" s="18" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F37" s="18" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G37" s="20"/>
       <c r="H37" s="20"/>
@@ -4297,15 +4430,15 @@
       <c r="J37" s="20"/>
     </row>
     <row r="38" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A38" s="28"/>
-      <c r="B38" s="28"/>
-      <c r="C38" s="29"/>
+      <c r="A38" s="37"/>
+      <c r="B38" s="37"/>
+      <c r="C38" s="24"/>
       <c r="D38" s="22" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E38" s="20"/>
       <c r="F38" s="22" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G38" s="20"/>
       <c r="H38" s="20"/>
@@ -4313,15 +4446,15 @@
       <c r="J38" s="20"/>
     </row>
     <row r="39" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A39" s="28"/>
-      <c r="B39" s="28"/>
-      <c r="C39" s="29"/>
+      <c r="A39" s="37"/>
+      <c r="B39" s="37"/>
+      <c r="C39" s="24"/>
       <c r="D39" s="20" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E39" s="20"/>
       <c r="F39" s="22" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="G39" s="20"/>
       <c r="H39" s="20"/>
@@ -4329,17 +4462,17 @@
       <c r="J39" s="20"/>
     </row>
     <row r="40" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A40" s="28"/>
-      <c r="B40" s="28"/>
-      <c r="C40" s="32" t="s">
-        <v>156</v>
+      <c r="A40" s="37"/>
+      <c r="B40" s="37"/>
+      <c r="C40" s="25" t="s">
+        <v>153</v>
       </c>
       <c r="D40" s="19" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="E40" s="19"/>
       <c r="F40" s="18" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="G40" s="20"/>
       <c r="H40" s="20"/>
@@ -4347,20 +4480,20 @@
       <c r="J40" s="20"/>
     </row>
     <row r="41" spans="1:10" ht="72" x14ac:dyDescent="0.3">
-      <c r="A41" s="28" t="s">
-        <v>108</v>
-      </c>
-      <c r="B41" s="28" t="s">
-        <v>158</v>
-      </c>
-      <c r="C41" s="36" t="s">
+      <c r="A41" s="37" t="s">
+        <v>106</v>
+      </c>
+      <c r="B41" s="37" t="s">
+        <v>155</v>
+      </c>
+      <c r="C41" s="41" t="s">
         <v>56</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>60</v>
+        <v>177</v>
       </c>
       <c r="E41" s="18" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F41" s="18" t="s">
         <v>55</v>
@@ -4371,15 +4504,15 @@
       <c r="J41" s="20"/>
     </row>
     <row r="42" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A42" s="28"/>
-      <c r="B42" s="28"/>
-      <c r="C42" s="36"/>
+      <c r="A42" s="37"/>
+      <c r="B42" s="37"/>
+      <c r="C42" s="41"/>
       <c r="D42" s="18" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E42" s="19"/>
       <c r="F42" s="18" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G42" s="20"/>
       <c r="H42" s="20"/>
@@ -4387,17 +4520,17 @@
       <c r="J42" s="20"/>
     </row>
     <row r="43" spans="1:10" ht="72" x14ac:dyDescent="0.3">
-      <c r="A43" s="28"/>
-      <c r="B43" s="28"/>
-      <c r="C43" s="36"/>
+      <c r="A43" s="37"/>
+      <c r="B43" s="37"/>
+      <c r="C43" s="41"/>
       <c r="D43" s="18" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E43" s="18" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F43" s="18" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G43" s="20"/>
       <c r="H43" s="20"/>
@@ -4405,15 +4538,15 @@
       <c r="J43" s="20"/>
     </row>
     <row r="44" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A44" s="28"/>
-      <c r="B44" s="28"/>
-      <c r="C44" s="36"/>
+      <c r="A44" s="37"/>
+      <c r="B44" s="37"/>
+      <c r="C44" s="41"/>
       <c r="D44" s="22" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E44" s="20"/>
       <c r="F44" s="22" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G44" s="20"/>
       <c r="H44" s="20"/>
@@ -4421,15 +4554,15 @@
       <c r="J44" s="20"/>
     </row>
     <row r="45" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A45" s="28"/>
-      <c r="B45" s="28"/>
-      <c r="C45" s="36"/>
+      <c r="A45" s="37"/>
+      <c r="B45" s="37"/>
+      <c r="C45" s="41"/>
       <c r="D45" s="20" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E45" s="20"/>
       <c r="F45" s="22" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="G45" s="20"/>
       <c r="H45" s="20"/>
@@ -4437,15 +4570,15 @@
       <c r="J45" s="20"/>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A46" s="28"/>
-      <c r="B46" s="28"/>
-      <c r="C46" s="36"/>
+      <c r="A46" s="37"/>
+      <c r="B46" s="37"/>
+      <c r="C46" s="41"/>
       <c r="D46" s="20" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="E46" s="20"/>
       <c r="F46" s="22" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="G46" s="20"/>
       <c r="H46" s="20"/>
@@ -4453,15 +4586,15 @@
       <c r="J46" s="20"/>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A47" s="28"/>
-      <c r="B47" s="28"/>
-      <c r="C47" s="36"/>
+      <c r="A47" s="37"/>
+      <c r="B47" s="37"/>
+      <c r="C47" s="41"/>
       <c r="D47" s="20" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E47" s="20"/>
       <c r="F47" s="22" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="G47" s="20"/>
       <c r="H47" s="20"/>
@@ -4469,15 +4602,15 @@
       <c r="J47" s="20"/>
     </row>
     <row r="48" spans="1:10" s="1" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A48" s="28"/>
-      <c r="B48" s="28"/>
-      <c r="C48" s="36"/>
-      <c r="D48" s="37" t="s">
-        <v>162</v>
+      <c r="A48" s="37"/>
+      <c r="B48" s="37"/>
+      <c r="C48" s="41"/>
+      <c r="D48" s="18" t="s">
+        <v>159</v>
       </c>
       <c r="E48" s="19"/>
       <c r="F48" s="18" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="G48" s="19"/>
       <c r="H48" s="19"/>
@@ -4485,22 +4618,22 @@
       <c r="J48" s="19"/>
     </row>
     <row r="49" spans="1:10" ht="72" x14ac:dyDescent="0.3">
-      <c r="A49" s="40" t="s">
-        <v>112</v>
-      </c>
-      <c r="B49" s="40" t="s">
-        <v>163</v>
-      </c>
-      <c r="C49" s="40" t="s">
+      <c r="A49" s="42" t="s">
+        <v>110</v>
+      </c>
+      <c r="B49" s="42" t="s">
+        <v>183</v>
+      </c>
+      <c r="C49" s="42" t="s">
         <v>56</v>
       </c>
-      <c r="D49" s="41" t="s">
-        <v>60</v>
-      </c>
-      <c r="E49" s="39" t="s">
-        <v>62</v>
-      </c>
-      <c r="F49" s="39" t="s">
+      <c r="D49" s="31" t="s">
+        <v>177</v>
+      </c>
+      <c r="E49" s="30" t="s">
+        <v>61</v>
+      </c>
+      <c r="F49" s="30" t="s">
         <v>55</v>
       </c>
       <c r="G49" s="20"/>
@@ -4509,15 +4642,15 @@
       <c r="J49" s="20"/>
     </row>
     <row r="50" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A50" s="40"/>
-      <c r="B50" s="40"/>
-      <c r="C50" s="40"/>
-      <c r="D50" s="39" t="s">
+      <c r="A50" s="42"/>
+      <c r="B50" s="42"/>
+      <c r="C50" s="42"/>
+      <c r="D50" s="30" t="s">
+        <v>65</v>
+      </c>
+      <c r="E50" s="32"/>
+      <c r="F50" s="30" t="s">
         <v>66</v>
-      </c>
-      <c r="E50" s="42"/>
-      <c r="F50" s="39" t="s">
-        <v>67</v>
       </c>
       <c r="G50" s="20"/>
       <c r="H50" s="20"/>
@@ -4525,17 +4658,17 @@
       <c r="J50" s="20"/>
     </row>
     <row r="51" spans="1:10" ht="72" x14ac:dyDescent="0.3">
-      <c r="A51" s="40"/>
-      <c r="B51" s="40"/>
-      <c r="C51" s="40"/>
-      <c r="D51" s="39" t="s">
-        <v>72</v>
-      </c>
-      <c r="E51" s="39" t="s">
+      <c r="A51" s="42"/>
+      <c r="B51" s="42"/>
+      <c r="C51" s="42"/>
+      <c r="D51" s="30" t="s">
         <v>71</v>
       </c>
-      <c r="F51" s="39" t="s">
-        <v>68</v>
+      <c r="E51" s="30" t="s">
+        <v>70</v>
+      </c>
+      <c r="F51" s="30" t="s">
+        <v>67</v>
       </c>
       <c r="G51" s="20"/>
       <c r="H51" s="20"/>
@@ -4543,15 +4676,15 @@
       <c r="J51" s="20"/>
     </row>
     <row r="52" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A52" s="40"/>
-      <c r="B52" s="40"/>
-      <c r="C52" s="40"/>
-      <c r="D52" s="43" t="s">
+      <c r="A52" s="42"/>
+      <c r="B52" s="42"/>
+      <c r="C52" s="42"/>
+      <c r="D52" s="33" t="s">
+        <v>68</v>
+      </c>
+      <c r="E52" s="34"/>
+      <c r="F52" s="33" t="s">
         <v>69</v>
-      </c>
-      <c r="E52" s="44"/>
-      <c r="F52" s="43" t="s">
-        <v>70</v>
       </c>
       <c r="G52" s="20"/>
       <c r="H52" s="20"/>
@@ -4559,15 +4692,15 @@
       <c r="J52" s="20"/>
     </row>
     <row r="53" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A53" s="40"/>
-      <c r="B53" s="40"/>
-      <c r="C53" s="40"/>
-      <c r="D53" s="44" t="s">
-        <v>83</v>
-      </c>
-      <c r="E53" s="44"/>
-      <c r="F53" s="43" t="s">
-        <v>84</v>
+      <c r="A53" s="42"/>
+      <c r="B53" s="42"/>
+      <c r="C53" s="42"/>
+      <c r="D53" s="34" t="s">
+        <v>81</v>
+      </c>
+      <c r="E53" s="34"/>
+      <c r="F53" s="33" t="s">
+        <v>82</v>
       </c>
       <c r="G53" s="20"/>
       <c r="H53" s="20"/>
@@ -4575,15 +4708,15 @@
       <c r="J53" s="20"/>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A54" s="40"/>
-      <c r="B54" s="40"/>
-      <c r="C54" s="40"/>
-      <c r="D54" s="44" t="s">
-        <v>134</v>
-      </c>
-      <c r="E54" s="44"/>
-      <c r="F54" s="43" t="s">
-        <v>140</v>
+      <c r="A54" s="42"/>
+      <c r="B54" s="42"/>
+      <c r="C54" s="42"/>
+      <c r="D54" s="34" t="s">
+        <v>131</v>
+      </c>
+      <c r="E54" s="34"/>
+      <c r="F54" s="33" t="s">
+        <v>137</v>
       </c>
       <c r="G54" s="20"/>
       <c r="H54" s="20"/>
@@ -4591,15 +4724,15 @@
       <c r="J54" s="20"/>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A55" s="40"/>
-      <c r="B55" s="40"/>
-      <c r="C55" s="40"/>
-      <c r="D55" s="44" t="s">
-        <v>87</v>
-      </c>
-      <c r="E55" s="44"/>
-      <c r="F55" s="43" t="s">
-        <v>92</v>
+      <c r="A55" s="42"/>
+      <c r="B55" s="42"/>
+      <c r="C55" s="42"/>
+      <c r="D55" s="34" t="s">
+        <v>85</v>
+      </c>
+      <c r="E55" s="34"/>
+      <c r="F55" s="33" t="s">
+        <v>90</v>
       </c>
       <c r="G55" s="20"/>
       <c r="H55" s="20"/>
@@ -4607,17 +4740,17 @@
       <c r="J55" s="20"/>
     </row>
     <row r="56" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A56" s="40"/>
-      <c r="B56" s="40"/>
-      <c r="C56" s="40"/>
-      <c r="D56" s="43" t="s">
-        <v>164</v>
-      </c>
-      <c r="E56" s="45" t="s">
-        <v>165</v>
-      </c>
-      <c r="F56" s="43" t="s">
-        <v>91</v>
+      <c r="A56" s="42"/>
+      <c r="B56" s="42"/>
+      <c r="C56" s="42"/>
+      <c r="D56" s="33" t="s">
+        <v>160</v>
+      </c>
+      <c r="E56" s="35" t="s">
+        <v>161</v>
+      </c>
+      <c r="F56" s="33" t="s">
+        <v>89</v>
       </c>
       <c r="G56" s="20"/>
       <c r="H56" s="20"/>
@@ -4625,15 +4758,15 @@
       <c r="J56" s="20"/>
     </row>
     <row r="57" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A57" s="40"/>
-      <c r="B57" s="40"/>
-      <c r="C57" s="40"/>
-      <c r="D57" s="44" t="s">
-        <v>89</v>
-      </c>
-      <c r="E57" s="44"/>
-      <c r="F57" s="43" t="s">
-        <v>166</v>
+      <c r="A57" s="42"/>
+      <c r="B57" s="42"/>
+      <c r="C57" s="42"/>
+      <c r="D57" s="34" t="s">
+        <v>87</v>
+      </c>
+      <c r="E57" s="34"/>
+      <c r="F57" s="33" t="s">
+        <v>162</v>
       </c>
       <c r="G57" s="20"/>
       <c r="H57" s="20"/>
@@ -4641,20 +4774,20 @@
       <c r="J57" s="20"/>
     </row>
     <row r="58" spans="1:10" ht="72" x14ac:dyDescent="0.3">
-      <c r="A58" s="28" t="s">
-        <v>119</v>
-      </c>
-      <c r="B58" s="28" t="s">
-        <v>167</v>
-      </c>
-      <c r="C58" s="28" t="s">
+      <c r="A58" s="37" t="s">
+        <v>116</v>
+      </c>
+      <c r="B58" s="37" t="s">
+        <v>163</v>
+      </c>
+      <c r="C58" s="37" t="s">
         <v>56</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>60</v>
+        <v>177</v>
       </c>
       <c r="E58" s="18" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F58" s="18" t="s">
         <v>55</v>
@@ -4665,15 +4798,15 @@
       <c r="J58" s="20"/>
     </row>
     <row r="59" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A59" s="28"/>
-      <c r="B59" s="28"/>
-      <c r="C59" s="28"/>
+      <c r="A59" s="37"/>
+      <c r="B59" s="37"/>
+      <c r="C59" s="37"/>
       <c r="D59" s="18" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E59" s="19"/>
       <c r="F59" s="18" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G59" s="20"/>
       <c r="H59" s="20"/>
@@ -4681,17 +4814,17 @@
       <c r="J59" s="20"/>
     </row>
     <row r="60" spans="1:10" ht="72" x14ac:dyDescent="0.3">
-      <c r="A60" s="28"/>
-      <c r="B60" s="28"/>
-      <c r="C60" s="28"/>
+      <c r="A60" s="37"/>
+      <c r="B60" s="37"/>
+      <c r="C60" s="37"/>
       <c r="D60" s="18" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E60" s="18" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F60" s="18" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G60" s="20"/>
       <c r="H60" s="20"/>
@@ -4699,15 +4832,15 @@
       <c r="J60" s="20"/>
     </row>
     <row r="61" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A61" s="28"/>
-      <c r="B61" s="28"/>
-      <c r="C61" s="28"/>
+      <c r="A61" s="37"/>
+      <c r="B61" s="37"/>
+      <c r="C61" s="37"/>
       <c r="D61" s="22" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E61" s="20"/>
       <c r="F61" s="22" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G61" s="20"/>
       <c r="H61" s="20"/>
@@ -4715,15 +4848,15 @@
       <c r="J61" s="20"/>
     </row>
     <row r="62" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A62" s="28"/>
-      <c r="B62" s="28"/>
-      <c r="C62" s="28"/>
+      <c r="A62" s="37"/>
+      <c r="B62" s="37"/>
+      <c r="C62" s="37"/>
       <c r="D62" s="20" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E62" s="20"/>
       <c r="F62" s="22" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="G62" s="20"/>
       <c r="H62" s="20"/>
@@ -4731,15 +4864,15 @@
       <c r="J62" s="20"/>
     </row>
     <row r="63" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A63" s="28"/>
-      <c r="B63" s="28"/>
-      <c r="C63" s="28"/>
+      <c r="A63" s="37"/>
+      <c r="B63" s="37"/>
+      <c r="C63" s="37"/>
       <c r="D63" s="20" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="E63" s="20"/>
       <c r="F63" s="22" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="G63" s="20"/>
       <c r="H63" s="20"/>
@@ -4747,15 +4880,15 @@
       <c r="J63" s="20"/>
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A64" s="28"/>
-      <c r="B64" s="28"/>
+      <c r="A64" s="37"/>
+      <c r="B64" s="37"/>
       <c r="C64" s="19"/>
       <c r="D64" s="19" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E64" s="19"/>
       <c r="F64" s="18" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="G64" s="20"/>
       <c r="H64" s="20"/>
@@ -4763,19 +4896,19 @@
       <c r="J64" s="20"/>
     </row>
     <row r="65" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A65" s="28"/>
-      <c r="B65" s="28"/>
-      <c r="C65" s="32" t="s">
-        <v>156</v>
+      <c r="A65" s="37"/>
+      <c r="B65" s="37"/>
+      <c r="C65" s="25" t="s">
+        <v>153</v>
       </c>
       <c r="D65" s="18" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="E65" s="18" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="F65" s="22" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="G65" s="20"/>
       <c r="H65" s="20"/>
@@ -4783,117 +4916,226 @@
       <c r="J65" s="20"/>
     </row>
     <row r="66" spans="1:10" ht="72" x14ac:dyDescent="0.3">
-      <c r="A66" s="28" t="s">
-        <v>124</v>
-      </c>
-      <c r="B66" s="28" t="s">
-        <v>171</v>
-      </c>
-      <c r="C66" s="28" t="s">
+      <c r="A66" s="37" t="s">
+        <v>121</v>
+      </c>
+      <c r="B66" s="37" t="s">
+        <v>167</v>
+      </c>
+      <c r="C66" s="37" t="s">
         <v>56</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>60</v>
+        <v>177</v>
       </c>
       <c r="E66" s="18" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F66" s="18" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="67" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A67" s="28"/>
-      <c r="B67" s="28"/>
-      <c r="C67" s="28"/>
+      <c r="A67" s="37"/>
+      <c r="B67" s="37"/>
+      <c r="C67" s="37"/>
       <c r="D67" s="18" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E67" s="19"/>
       <c r="F67" s="18" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10" ht="72" x14ac:dyDescent="0.3">
+      <c r="A68" s="37"/>
+      <c r="B68" s="37"/>
+      <c r="C68" s="37"/>
+      <c r="D68" s="18" t="s">
+        <v>71</v>
+      </c>
+      <c r="E68" s="18" t="s">
+        <v>70</v>
+      </c>
+      <c r="F68" s="18" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="68" spans="1:10" ht="72" x14ac:dyDescent="0.3">
-      <c r="A68" s="28"/>
-      <c r="B68" s="28"/>
-      <c r="C68" s="28"/>
-      <c r="D68" s="18" t="s">
-        <v>72</v>
-      </c>
-      <c r="E68" s="18" t="s">
-        <v>71</v>
-      </c>
-      <c r="F68" s="18" t="s">
+    <row r="69" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A69" s="37"/>
+      <c r="B69" s="37"/>
+      <c r="C69" s="37"/>
+      <c r="D69" s="22" t="s">
         <v>68</v>
-      </c>
-    </row>
-    <row r="69" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A69" s="28"/>
-      <c r="B69" s="28"/>
-      <c r="C69" s="28"/>
-      <c r="D69" s="22" t="s">
-        <v>69</v>
       </c>
       <c r="E69" s="20"/>
       <c r="F69" s="22" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="70" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A70" s="28"/>
-      <c r="B70" s="28"/>
-      <c r="C70" s="28"/>
+      <c r="A70" s="37"/>
+      <c r="B70" s="37"/>
+      <c r="C70" s="37"/>
       <c r="D70" s="20" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E70" s="20"/>
       <c r="F70" s="22" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="71" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A71" s="28"/>
-      <c r="B71" s="28"/>
-      <c r="C71" s="28"/>
+      <c r="A71" s="37"/>
+      <c r="B71" s="37"/>
+      <c r="C71" s="37"/>
       <c r="D71" s="20" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="E71" s="20"/>
       <c r="F71" s="22" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
     </row>
     <row r="72" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A72" s="28"/>
-      <c r="B72" s="28"/>
+      <c r="A72" s="37"/>
+      <c r="B72" s="37"/>
       <c r="C72" s="19"/>
       <c r="D72" s="19" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E72" s="19"/>
       <c r="F72" s="18" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="73" spans="1:10" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A73" s="28"/>
-      <c r="B73" s="28"/>
-      <c r="C73" s="32" t="s">
-        <v>172</v>
+      <c r="A73" s="37"/>
+      <c r="B73" s="37"/>
+      <c r="C73" s="25" t="s">
+        <v>168</v>
       </c>
       <c r="D73" s="18" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="E73" s="18" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="F73" s="18" t="s">
-        <v>173</v>
-      </c>
+        <v>169</v>
+      </c>
+    </row>
+    <row r="74" spans="1:10" ht="72" x14ac:dyDescent="0.3">
+      <c r="A74" s="37" t="s">
+        <v>126</v>
+      </c>
+      <c r="B74" s="37" t="s">
+        <v>184</v>
+      </c>
+      <c r="C74" s="37" t="s">
+        <v>56</v>
+      </c>
+      <c r="D74" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="E74" s="18" t="s">
+        <v>61</v>
+      </c>
+      <c r="F74" s="18" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="75" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A75" s="37"/>
+      <c r="B75" s="37"/>
+      <c r="C75" s="37"/>
+      <c r="D75" s="18" t="s">
+        <v>65</v>
+      </c>
+      <c r="E75" s="19"/>
+      <c r="F75" s="18" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="76" spans="1:10" ht="72" x14ac:dyDescent="0.3">
+      <c r="A76" s="37"/>
+      <c r="B76" s="37"/>
+      <c r="C76" s="37"/>
+      <c r="D76" s="18" t="s">
+        <v>71</v>
+      </c>
+      <c r="E76" s="18" t="s">
+        <v>70</v>
+      </c>
+      <c r="F76" s="18" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A77" s="37"/>
+      <c r="B77" s="37"/>
+      <c r="C77" s="37"/>
+      <c r="D77" s="22" t="s">
+        <v>68</v>
+      </c>
+      <c r="E77" s="20"/>
+      <c r="F77" s="22" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A78" s="37"/>
+      <c r="B78" s="37"/>
+      <c r="C78" s="37"/>
+      <c r="D78" s="20" t="s">
+        <v>81</v>
+      </c>
+      <c r="E78" s="20"/>
+      <c r="F78" s="22" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A79" s="37"/>
+      <c r="B79" s="37"/>
+      <c r="C79" s="37"/>
+      <c r="D79" s="20" t="s">
+        <v>131</v>
+      </c>
+      <c r="E79" s="20"/>
+      <c r="F79" s="22" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A80" s="37"/>
+      <c r="B80" s="37"/>
+      <c r="C80" s="25" t="s">
+        <v>153</v>
+      </c>
+      <c r="D80" s="22" t="s">
+        <v>185</v>
+      </c>
+      <c r="E80" s="18" t="s">
+        <v>186</v>
+      </c>
+      <c r="F80" s="22" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A81" s="37"/>
+      <c r="B81" s="37"/>
+      <c r="C81" s="24"/>
+      <c r="D81" s="20"/>
+      <c r="E81" s="20"/>
+      <c r="F81" s="20"/>
     </row>
   </sheetData>
-  <mergeCells count="26">
+  <mergeCells count="29">
+    <mergeCell ref="A74:A81"/>
+    <mergeCell ref="B74:B81"/>
+    <mergeCell ref="C74:C79"/>
     <mergeCell ref="C58:C63"/>
     <mergeCell ref="A58:A65"/>
     <mergeCell ref="B58:B65"/>
@@ -4939,6 +5181,32 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F07F0BC-B2D7-405D-8351-BA7CCDA175A2}">
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="82.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="273.60000000000002" x14ac:dyDescent="0.3">
+      <c r="A1" s="29" t="s">
+        <v>176</v>
+      </c>
+      <c r="B1" t="s">
+        <v>189</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5F67A5B-0CD8-4428-B317-0FA6EE971711}">
   <dimension ref="A1"/>
   <sheetViews>

</xml_diff>